<commit_message>
adds joblib parallel backend
</commit_message>
<xml_diff>
--- a/src/regression_analysis/cv_results.xlsx
+++ b/src/regression_analysis/cv_results.xlsx
@@ -813,19 +813,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1.051401853561401</v>
+        <v>1.489297008514404</v>
       </c>
       <c r="C2">
-        <v>0.05079960823059082</v>
+        <v>0.1286006450653076</v>
       </c>
       <c r="D2">
-        <v>-2.891742282571763E+28</v>
+        <v>-8.232647213133496E+27</v>
       </c>
       <c r="E2">
-        <v>-79911605353267.53</v>
+        <v>-49419033809451.61</v>
       </c>
       <c r="F2">
-        <v>-4.317574468258415E+24</v>
+        <v>-1.241948841029304E+24</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -843,64 +843,64 @@
         <v>71</v>
       </c>
       <c r="P2">
-        <v>-5623.813548025984</v>
+        <v>-5720.244016060848</v>
       </c>
       <c r="Q2">
-        <v>-74.99208990304234</v>
+        <v>-75.63229479568135</v>
       </c>
       <c r="R2">
-        <v>0.6369389107002398</v>
+        <v>0.6307135708187794</v>
       </c>
       <c r="S2">
-        <v>-2.045329092480589E+25</v>
+        <v>-1.377594850601338E+26</v>
       </c>
       <c r="T2">
-        <v>-4522531473058.633</v>
+        <v>-11737098664496.85</v>
       </c>
       <c r="U2">
-        <v>-3.433847786401327E+21</v>
+        <v>-2.312806797539925E+22</v>
       </c>
       <c r="V2">
-        <v>-1.443381402185695E+29</v>
+        <v>-3.972635256099746E+28</v>
       </c>
       <c r="W2">
-        <v>-379918596831702.2</v>
+        <v>-199314707337410.2</v>
       </c>
       <c r="X2">
-        <v>-2.153898194951742E+25</v>
+        <v>-5.928198807576195E+24</v>
       </c>
       <c r="Y2">
-        <v>-2.285206190938127E+26</v>
+        <v>-1.299124019609885E+27</v>
       </c>
       <c r="Z2">
-        <v>-15116898461450.77</v>
+        <v>-36043363045224.91</v>
       </c>
       <c r="AA2">
-        <v>-4.545654398826056E+22</v>
+        <v>-2.584173295949271E+23</v>
       </c>
       <c r="AB2">
-        <v>-2605.926386300865</v>
+        <v>-2551.17455263899</v>
       </c>
       <c r="AC2">
-        <v>-51.04827505705619</v>
+        <v>-50.5091531570169</v>
       </c>
       <c r="AD2">
-        <v>0.526166461277483</v>
+        <v>0.536121943992549</v>
       </c>
       <c r="AE2">
-        <v>0.09742213777851542</v>
+        <v>0.3983333902049447</v>
       </c>
       <c r="AF2">
-        <v>0.003385943872698211</v>
+        <v>0.1279216346187257</v>
       </c>
       <c r="AG2">
-        <v>5.771042305746722E+28</v>
+        <v>1.575441136961421E+28</v>
       </c>
       <c r="AH2">
-        <v>150105156991960.9</v>
+        <v>76094719333694.75</v>
       </c>
       <c r="AI2">
-        <v>8.610720934573996E+24</v>
+        <v>2.345151206521273E+24</v>
       </c>
     </row>
     <row r="3" spans="1:35">
@@ -908,19 +908,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.180699014663696</v>
+        <v>1.430600309371948</v>
       </c>
       <c r="C3">
-        <v>0.04010109901428223</v>
+        <v>0.223100471496582</v>
       </c>
       <c r="D3">
-        <v>-3.908388502460945E+27</v>
+        <v>-1.780917253390365E+27</v>
       </c>
       <c r="E3">
-        <v>-34579923789097.7</v>
+        <v>-29019692008883.23</v>
       </c>
       <c r="F3">
-        <v>-5.869446902787182E+23</v>
+        <v>-2.955327839614086E+23</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
@@ -938,64 +938,64 @@
         <v>70</v>
       </c>
       <c r="P3">
-        <v>-9059.421455501433</v>
+        <v>-9142.829679554088</v>
       </c>
       <c r="Q3">
-        <v>-95.18099314202092</v>
+        <v>-95.61814513759451</v>
       </c>
       <c r="R3">
-        <v>0.4151435864699879</v>
+        <v>0.4097589341477671</v>
       </c>
       <c r="S3">
-        <v>-4.444206972346402E+26</v>
+        <v>-6.718851546869011E+27</v>
       </c>
       <c r="T3">
-        <v>-21081287845732.77</v>
+        <v>-81968600981528.36</v>
       </c>
       <c r="U3">
-        <v>-7.461259085594249E+22</v>
+        <v>-1.128009844293272E+24</v>
       </c>
       <c r="V3">
-        <v>-1.889090594321561E+28</v>
+        <v>-1.713092390455959E+27</v>
       </c>
       <c r="W3">
-        <v>-137444192104343.2</v>
+        <v>-41389520297485.43</v>
       </c>
       <c r="X3">
-        <v>-2.819011534337372E+24</v>
+        <v>-2.556376715122693E+23</v>
       </c>
       <c r="Y3">
-        <v>-2.066158718544759E+26</v>
+        <v>-4.726423296268572E+26</v>
       </c>
       <c r="Z3">
-        <v>-14374138995239.88</v>
+        <v>-21740338765227.58</v>
       </c>
       <c r="AA3">
-        <v>-4.109932620027671E+22</v>
+        <v>-9.401640400150169E+22</v>
       </c>
       <c r="AB3">
-        <v>-5995.537668794373</v>
+        <v>-6260.214872628674</v>
       </c>
       <c r="AC3">
-        <v>-77.43085734249863</v>
+        <v>-79.12151965570855</v>
       </c>
       <c r="AD3">
-        <v>-0.09016388378554763</v>
+        <v>-0.1382899309261241</v>
       </c>
       <c r="AE3">
-        <v>0.01925280429640894</v>
+        <v>0.2527656397922368</v>
       </c>
       <c r="AF3">
-        <v>0.006530250896018631</v>
+        <v>0.2453181145200548</v>
       </c>
       <c r="AG3">
-        <v>7.493050430888705E+27</v>
+        <v>2.54726171021903E+27</v>
       </c>
       <c r="AH3">
-        <v>52082793446599.43</v>
+        <v>30639430952612.75</v>
       </c>
       <c r="AI3">
-        <v>1.116383614786924E+24</v>
+        <v>4.265906187811019E+23</v>
       </c>
     </row>
     <row r="4" spans="1:35">
@@ -1003,10 +1003,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.6201006412506104</v>
+        <v>0.512399435043335</v>
       </c>
       <c r="C4">
-        <v>0.05950069427490234</v>
+        <v>0.03820013999938965</v>
       </c>
       <c r="D4">
         <v>-5164.379142546594</v>
@@ -1084,10 +1084,10 @@
         <v>0.3511237074601231</v>
       </c>
       <c r="AE4">
-        <v>0.07038249545089235</v>
+        <v>0.3786305738583262</v>
       </c>
       <c r="AF4">
-        <v>0.01030603558260089</v>
+        <v>0.00461029824053027</v>
       </c>
       <c r="AG4">
         <v>2385.557212318412</v>
@@ -1104,10 +1104,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.5367039680480957</v>
+        <v>0.3471000671386719</v>
       </c>
       <c r="C5">
-        <v>0.04999842643737793</v>
+        <v>0.0380007266998291</v>
       </c>
       <c r="D5">
         <v>-5164.379142546594</v>
@@ -1185,10 +1185,10 @@
         <v>0.3511237074601231</v>
       </c>
       <c r="AE5">
-        <v>0.02008428526467862</v>
+        <v>0.02201190342996293</v>
       </c>
       <c r="AF5">
-        <v>0.007347424608650986</v>
+        <v>0.01163630710098371</v>
       </c>
       <c r="AG5">
         <v>2385.557212318412</v>
@@ -1205,10 +1205,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.5788066864013672</v>
+        <v>0.3292991161346436</v>
       </c>
       <c r="C6">
-        <v>0.05189599990844727</v>
+        <v>0.03250126838684082</v>
       </c>
       <c r="D6">
         <v>-5164.379142546594</v>
@@ -1286,10 +1286,10 @@
         <v>0.3511237074601231</v>
       </c>
       <c r="AE6">
-        <v>0.02070959937730527</v>
+        <v>0.003708509265337785</v>
       </c>
       <c r="AF6">
-        <v>0.003549737610811036</v>
+        <v>0.002301531375660443</v>
       </c>
       <c r="AG6">
         <v>2385.557212318412</v>
@@ -1306,10 +1306,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.5953993797302246</v>
+        <v>0.3474982738494873</v>
       </c>
       <c r="C7">
-        <v>0.05950484275817871</v>
+        <v>0.03690128326416016</v>
       </c>
       <c r="D7">
         <v>-5164.379142546594</v>
@@ -1387,10 +1387,10 @@
         <v>0.3511237074601231</v>
       </c>
       <c r="AE7">
-        <v>0.03296813628233081</v>
+        <v>0.01318833789230831</v>
       </c>
       <c r="AF7">
-        <v>0.008381940916196822</v>
+        <v>0.01115167553003442</v>
       </c>
       <c r="AG7">
         <v>2385.557212318412</v>
@@ -1407,10 +1407,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.5761006355285645</v>
+        <v>0.3453980922698975</v>
       </c>
       <c r="C8">
-        <v>0.05550017356872559</v>
+        <v>0.03090105056762695</v>
       </c>
       <c r="D8">
         <v>-5164.379142546594</v>
@@ -1488,10 +1488,10 @@
         <v>0.3511237074601231</v>
       </c>
       <c r="AE8">
-        <v>0.02188001776784539</v>
+        <v>0.003838949473583193</v>
       </c>
       <c r="AF8">
-        <v>0.007198720870362713</v>
+        <v>0.008256011938262038</v>
       </c>
       <c r="AG8">
         <v>2385.557212318412</v>
@@ -1508,19 +1508,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.5946011066436767</v>
+        <v>0.3185001850128174</v>
       </c>
       <c r="C9">
-        <v>0.06530189514160156</v>
+        <v>0.03090114593505859</v>
       </c>
       <c r="D9">
-        <v>-3471.57943776676</v>
+        <v>-3706.868041217938</v>
       </c>
       <c r="E9">
-        <v>-58.06186283225433</v>
+        <v>-59.52380191161012</v>
       </c>
       <c r="F9">
-        <v>0.5186277135688468</v>
+        <v>0.4950246382205202</v>
       </c>
       <c r="G9" t="s">
         <v>34</v>
@@ -1535,22 +1535,22 @@
         <v>44</v>
       </c>
       <c r="M9">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="N9">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O9">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="P9">
-        <v>-5813.767156707644</v>
+        <v>-6774.631921170455</v>
       </c>
       <c r="Q9">
-        <v>-76.24806329807757</v>
+        <v>-82.30815221574625</v>
       </c>
       <c r="R9">
-        <v>0.6246759216278885</v>
+        <v>0.562644596251165</v>
       </c>
       <c r="S9">
         <v>-2987.97710372402</v>
@@ -1562,22 +1562,22 @@
         <v>0.4983565920437351</v>
       </c>
       <c r="V9">
-        <v>-2695.477513958275</v>
+        <v>-2431.807513958275</v>
       </c>
       <c r="W9">
-        <v>-51.9179883466056</v>
+        <v>-49.31336040018238</v>
       </c>
       <c r="X9">
-        <v>0.5977650714456962</v>
+        <v>0.6371114518412684</v>
       </c>
       <c r="Y9">
-        <v>-3629.404126969922</v>
+        <v>-4108.652379763005</v>
       </c>
       <c r="Z9">
-        <v>-60.24453607564691</v>
+        <v>-64.09877050118048</v>
       </c>
       <c r="AA9">
-        <v>0.2780512804358599</v>
+        <v>0.1827208486753782</v>
       </c>
       <c r="AB9">
         <v>-2231.271287473935</v>
@@ -1589,19 +1589,19 @@
         <v>0.594289702291054</v>
       </c>
       <c r="AE9">
-        <v>0.0183836856061232</v>
+        <v>0.01249821188555772</v>
       </c>
       <c r="AF9">
-        <v>0.01002361230143971</v>
+        <v>0.004587443995577723</v>
       </c>
       <c r="AG9">
-        <v>1255.812220405041</v>
+        <v>1666.887829800663</v>
       </c>
       <c r="AH9">
-        <v>10.01995619826967</v>
+        <v>12.79785322643357</v>
       </c>
       <c r="AI9">
-        <v>0.12768838547694</v>
+        <v>0.162578862804749</v>
       </c>
     </row>
     <row r="10" spans="1:35">
@@ -1609,19 +1609,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.5968024253845214</v>
+        <v>0.3515985488891601</v>
       </c>
       <c r="C10">
-        <v>0.05520281791687012</v>
+        <v>0.03400106430053711</v>
       </c>
       <c r="D10">
-        <v>-3655.438877503108</v>
+        <v>-3658.120692317922</v>
       </c>
       <c r="E10">
-        <v>-58.99668892310647</v>
+        <v>-59.01808542927264</v>
       </c>
       <c r="F10">
-        <v>0.5070322168193002</v>
+        <v>0.5064987593414525</v>
       </c>
       <c r="G10" t="s">
         <v>34</v>
@@ -1636,13 +1636,13 @@
         <v>45</v>
       </c>
       <c r="M10">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N10">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O10">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P10">
         <v>-6861.107463213388</v>
@@ -1672,13 +1672,13 @@
         <v>0.6374338644317565</v>
       </c>
       <c r="Y10">
-        <v>-3920.759072846874</v>
+        <v>-3934.168146920948</v>
       </c>
       <c r="Z10">
-        <v>-62.6159649997257</v>
+        <v>-62.72294753055653</v>
       </c>
       <c r="AA10">
-        <v>0.2200959459633239</v>
+        <v>0.217428658574085</v>
       </c>
       <c r="AB10">
         <v>-2077.703801705267</v>
@@ -1690,19 +1690,19 @@
         <v>0.62221275706229</v>
       </c>
       <c r="AE10">
-        <v>0.01576703708922996</v>
+        <v>0.02434068846965416</v>
       </c>
       <c r="AF10">
-        <v>0.004217067581441577</v>
+        <v>0.005857433570065811</v>
       </c>
       <c r="AG10">
-        <v>1719.536270952174</v>
+        <v>1719.958381736022</v>
       </c>
       <c r="AH10">
-        <v>13.22231347432493</v>
+        <v>13.22823815105398</v>
       </c>
       <c r="AI10">
-        <v>0.1517773423201581</v>
+        <v>0.1527862446295507</v>
       </c>
     </row>
     <row r="11" spans="1:35">
@@ -1710,19 +1710,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.5814980030059814</v>
+        <v>0.3411983489990235</v>
       </c>
       <c r="C11">
-        <v>0.05199952125549316</v>
+        <v>0.02770066261291504</v>
       </c>
       <c r="D11">
-        <v>-3412.127234014262</v>
+        <v>-3414.809048829077</v>
       </c>
       <c r="E11">
-        <v>-57.32245980070638</v>
+        <v>-57.34733193696337</v>
       </c>
       <c r="F11">
-        <v>0.5430177478741409</v>
+        <v>0.5424842903962931</v>
       </c>
       <c r="G11" t="s">
         <v>34</v>
@@ -1737,13 +1737,13 @@
         <v>46</v>
       </c>
       <c r="M11">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N11">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O11">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="P11">
         <v>-6261.034743230151</v>
@@ -1773,13 +1773,13 @@
         <v>0.5786496261693499</v>
       </c>
       <c r="Y11">
-        <v>-2899.806530715354</v>
+        <v>-2913.215604789428</v>
       </c>
       <c r="Z11">
-        <v>-53.84985172417241</v>
+        <v>-53.97421240545737</v>
       </c>
       <c r="AA11">
-        <v>0.4231803517616294</v>
+        <v>0.4205130643723904</v>
       </c>
       <c r="AB11">
         <v>-2173.997478959378</v>
@@ -1791,19 +1791,19 @@
         <v>0.6047037537037234</v>
       </c>
       <c r="AE11">
-        <v>0.02734218157562179</v>
+        <v>0.007877540780321417</v>
       </c>
       <c r="AF11">
-        <v>0.004382502315137934</v>
+        <v>0.005006269870699915</v>
       </c>
       <c r="AG11">
-        <v>1450.386738472097</v>
+        <v>1449.449054349426</v>
       </c>
       <c r="AH11">
-        <v>11.23667372538078</v>
+        <v>11.22909473380724</v>
       </c>
       <c r="AI11">
-        <v>0.068026189064354</v>
+        <v>0.06896779695122916</v>
       </c>
     </row>
     <row r="12" spans="1:35">
@@ -1811,19 +1811,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.6273026943206788</v>
+        <v>0.3371997356414795</v>
       </c>
       <c r="C12">
-        <v>0.0501981258392334</v>
+        <v>0.03290185928344726</v>
       </c>
       <c r="D12">
-        <v>-3501.2532215123</v>
+        <v>-3498.571406697485</v>
       </c>
       <c r="E12">
-        <v>-58.16002053681596</v>
+        <v>-58.1362760724665</v>
       </c>
       <c r="F12">
-        <v>0.526066691956381</v>
+        <v>0.5266001494342288</v>
       </c>
       <c r="G12" t="s">
         <v>34</v>
@@ -1838,13 +1838,13 @@
         <v>47</v>
       </c>
       <c r="M12">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N12">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O12">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P12">
         <v>-6261.034743230151</v>
@@ -1874,13 +1874,13 @@
         <v>0.5750093728054271</v>
       </c>
       <c r="Y12">
-        <v>-3195.842490684308</v>
+        <v>-3182.433416610234</v>
       </c>
       <c r="Z12">
-        <v>-56.53178301348992</v>
+        <v>-56.41306069174259</v>
       </c>
       <c r="AA12">
-        <v>0.3642938858934821</v>
+        <v>0.3669611732827212</v>
       </c>
       <c r="AB12">
         <v>-2260.722810293703</v>
@@ -1892,19 +1892,19 @@
         <v>0.5889345551342432</v>
       </c>
       <c r="AE12">
-        <v>0.0179137409616373</v>
+        <v>0.01511805652817151</v>
       </c>
       <c r="AF12">
-        <v>0.004923697690727149</v>
+        <v>0.007003223532061378</v>
       </c>
       <c r="AG12">
-        <v>1413.47719547263</v>
+        <v>1414.066710126878</v>
       </c>
       <c r="AH12">
-        <v>10.89335727264301</v>
+        <v>10.8970092742662</v>
       </c>
       <c r="AI12">
-        <v>0.08691611729406536</v>
+        <v>0.08592410562109483</v>
       </c>
     </row>
     <row r="13" spans="1:35">
@@ -1912,10 +1912,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.5906006813049316</v>
+        <v>0.3582986831665039</v>
       </c>
       <c r="C13">
-        <v>0.0462984561920166</v>
+        <v>0.03250117301940918</v>
       </c>
       <c r="D13">
         <v>-3415.769398706841</v>
@@ -1993,10 +1993,10 @@
         <v>0.6057372707417165</v>
       </c>
       <c r="AE13">
-        <v>0.03772124624610075</v>
+        <v>0.01643926625843239</v>
       </c>
       <c r="AF13">
-        <v>0.005642994176926783</v>
+        <v>0.007687873946366561</v>
       </c>
       <c r="AG13">
         <v>1451.673145145337</v>
@@ -2013,19 +2013,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.6128010749816895</v>
+        <v>0.3335998058319092</v>
       </c>
       <c r="C14">
-        <v>0.04960198402404785</v>
+        <v>0.03560099601745605</v>
       </c>
       <c r="D14">
-        <v>-3204.666361521942</v>
+        <v>-3187.764051794027</v>
       </c>
       <c r="E14">
-        <v>-55.98081608185875</v>
+        <v>-55.79207944868349</v>
       </c>
       <c r="F14">
-        <v>0.54765097588782</v>
+        <v>0.5486543558849069</v>
       </c>
       <c r="G14" t="s">
         <v>34</v>
@@ -2043,70 +2043,70 @@
         <v>9</v>
       </c>
       <c r="N14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O14">
         <v>13</v>
       </c>
       <c r="P14">
-        <v>-5067.743321035088</v>
+        <v>-4978.630265479533</v>
       </c>
       <c r="Q14">
-        <v>-71.18808412252073</v>
+        <v>-70.55940947513331</v>
       </c>
       <c r="R14">
-        <v>0.6728375870369303</v>
+        <v>0.6785905307902285</v>
       </c>
       <c r="S14">
-        <v>-2863.241097900698</v>
+        <v>-2859.078347129092</v>
       </c>
       <c r="T14">
-        <v>-53.50926179551254</v>
+        <v>-53.47035016837923</v>
       </c>
       <c r="U14">
-        <v>0.5192981832554202</v>
+        <v>0.5199970562424114</v>
       </c>
       <c r="V14">
-        <v>-2312.049279813009</v>
+        <v>-2407.18347258523</v>
       </c>
       <c r="W14">
-        <v>-48.08377356045393</v>
+        <v>-49.06305608688915</v>
       </c>
       <c r="X14">
-        <v>0.6549824763650354</v>
+        <v>0.6407859953947258</v>
       </c>
       <c r="Y14">
-        <v>-3384.737804309074</v>
+        <v>-3556.970869224439</v>
       </c>
       <c r="Z14">
-        <v>-58.17849950204177</v>
+        <v>-59.64034598511681</v>
       </c>
       <c r="AA14">
-        <v>0.3267194728404723</v>
+        <v>0.2924594576059425</v>
       </c>
       <c r="AB14">
-        <v>-2395.560304551841</v>
+        <v>-2136.957304551841</v>
       </c>
       <c r="AC14">
-        <v>-48.94446142876475</v>
+        <v>-46.22723552789893</v>
       </c>
       <c r="AD14">
-        <v>0.5644171599412411</v>
+        <v>0.6114387393912263</v>
       </c>
       <c r="AE14">
-        <v>0.0377994842978706</v>
+        <v>0.01711647335298869</v>
       </c>
       <c r="AF14">
-        <v>0.005504717753466573</v>
+        <v>0.003930335844936713</v>
       </c>
       <c r="AG14">
-        <v>1007.121696539132</v>
+        <v>1016.371056504078</v>
       </c>
       <c r="AH14">
-        <v>8.415140660205703</v>
+        <v>8.660711436470846</v>
       </c>
       <c r="AI14">
-        <v>0.1241671884373793</v>
+        <v>0.1383984061230698</v>
       </c>
     </row>
     <row r="15" spans="1:35">
@@ -2114,19 +2114,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.597799825668335</v>
+        <v>0.3461999416351318</v>
       </c>
       <c r="C15">
-        <v>0.05460081100463867</v>
+        <v>0.03800220489501953</v>
       </c>
       <c r="D15">
-        <v>-3471.036621015627</v>
+        <v>-3473.705603561046</v>
       </c>
       <c r="E15">
-        <v>-57.46653437457085</v>
+        <v>-57.48843281978477</v>
       </c>
       <c r="F15">
-        <v>0.5274923868471809</v>
+        <v>0.5270637973184027</v>
       </c>
       <c r="G15" t="s">
         <v>34</v>
@@ -2150,13 +2150,13 @@
         <v>55</v>
       </c>
       <c r="P15">
-        <v>-6391.776872380846</v>
+        <v>-6395.204842442575</v>
       </c>
       <c r="Q15">
-        <v>-79.94858893301898</v>
+        <v>-79.97002464950586</v>
       </c>
       <c r="R15">
-        <v>0.5873608799384609</v>
+        <v>0.5871395776968289</v>
       </c>
       <c r="S15">
         <v>-2574.060781396647</v>
@@ -2177,37 +2177,37 @@
         <v>0.6468611003367144</v>
       </c>
       <c r="Y15">
-        <v>-4065.790020231099</v>
+        <v>-4072.722358452025</v>
       </c>
       <c r="Z15">
-        <v>-63.76354773874411</v>
+        <v>-63.81788431507287</v>
       </c>
       <c r="AA15">
-        <v>0.1912468833904463</v>
+        <v>0.1898679262594416</v>
       </c>
       <c r="AB15">
-        <v>-1957.082766033825</v>
+        <v>-1960.067370478269</v>
       </c>
       <c r="AC15">
-        <v>-44.23892817455939</v>
+        <v>-44.27264810781335</v>
       </c>
       <c r="AD15">
-        <v>0.6441451848073829</v>
+        <v>0.6436024965361283</v>
       </c>
       <c r="AE15">
-        <v>0.01407148675438534</v>
+        <v>0.01323015003455272</v>
       </c>
       <c r="AF15">
-        <v>0.009410958210320843</v>
+        <v>0.005448404674339204</v>
       </c>
       <c r="AG15">
-        <v>1624.877760728342</v>
+        <v>1626.063046888285</v>
       </c>
       <c r="AH15">
-        <v>12.98591729497356</v>
+        <v>12.99175490402046</v>
       </c>
       <c r="AI15">
-        <v>0.1709564894262398</v>
+        <v>0.1714095440419569</v>
       </c>
     </row>
     <row r="16" spans="1:35">
@@ -2215,19 +2215,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5964023113250733</v>
+        <v>0.3533985137939453</v>
       </c>
       <c r="C16">
-        <v>0.04699888229370117</v>
+        <v>0.03280096054077149</v>
       </c>
       <c r="D16">
-        <v>-3158.584480308727</v>
+        <v>-3157.314110392934</v>
       </c>
       <c r="E16">
-        <v>-55.1087727776821</v>
+        <v>-55.09478651688359</v>
       </c>
       <c r="F16">
-        <v>0.578452251258094</v>
+        <v>0.5787369180574881</v>
       </c>
       <c r="G16" t="s">
         <v>34</v>
@@ -2251,13 +2251,13 @@
         <v>5</v>
       </c>
       <c r="P16">
-        <v>-5840.558550408559</v>
+        <v>-5842.050183082169</v>
       </c>
       <c r="Q16">
-        <v>-76.42354709386734</v>
+        <v>-76.43330545699413</v>
       </c>
       <c r="R16">
-        <v>0.6229463279104142</v>
+        <v>0.6228500313709411</v>
       </c>
       <c r="S16">
         <v>-2601.834611034529</v>
@@ -2278,37 +2278,37 @@
         <v>0.5955185102929099</v>
       </c>
       <c r="Y16">
-        <v>-2674.58159402617</v>
+        <v>-2669.112276206479</v>
       </c>
       <c r="Z16">
-        <v>-51.71635712254074</v>
+        <v>-51.66345203532647</v>
       </c>
       <c r="AA16">
-        <v>0.467981329819816</v>
+        <v>0.4690692679106649</v>
       </c>
       <c r="AB16">
-        <v>-1965.415360287028</v>
+        <v>-1963.041195854146</v>
       </c>
       <c r="AC16">
-        <v>-44.33300531530688</v>
+        <v>-44.30622073540177</v>
       </c>
       <c r="AD16">
-        <v>0.6426300757688121</v>
+        <v>0.6430617682144067</v>
       </c>
       <c r="AE16">
-        <v>0.01434479631089403</v>
+        <v>0.01691815537245724</v>
       </c>
       <c r="AF16">
-        <v>0.005428891877522534</v>
+        <v>0.003487864693325011</v>
       </c>
       <c r="AG16">
-        <v>1368.328720852071</v>
+        <v>1369.715888665104</v>
       </c>
       <c r="AH16">
-        <v>11.027585558341</v>
+        <v>11.03986453956555</v>
       </c>
       <c r="AI16">
-        <v>0.06136234395177326</v>
+        <v>0.061047735759998</v>
       </c>
     </row>
     <row r="17" spans="1:35">
@@ -2316,19 +2316,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.6051003932952881</v>
+        <v>0.3217989444732666</v>
       </c>
       <c r="C17">
-        <v>0.04519991874694824</v>
+        <v>0.02990241050720215</v>
       </c>
       <c r="D17">
-        <v>-3250.473623139662</v>
+        <v>-3250.908712274625</v>
       </c>
       <c r="E17">
-        <v>-55.92444009069807</v>
+        <v>-55.92758584219142</v>
       </c>
       <c r="F17">
-        <v>0.5644696345301776</v>
+        <v>0.5643820298124715</v>
       </c>
       <c r="G17" t="s">
         <v>34</v>
@@ -2346,19 +2346,19 @@
         <v>13</v>
       </c>
       <c r="N17">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O17">
         <v>12</v>
       </c>
       <c r="P17">
-        <v>-5979.450548756079</v>
+        <v>-5980.431519417848</v>
       </c>
       <c r="Q17">
-        <v>-77.32690701661407</v>
+        <v>-77.33324976630588</v>
       </c>
       <c r="R17">
-        <v>0.613979764601648</v>
+        <v>0.6139164352835632</v>
       </c>
       <c r="S17">
         <v>-2714.043740401265</v>
@@ -2370,46 +2370,46 @@
         <v>0.5443465247506762</v>
       </c>
       <c r="V17">
-        <v>-2674.681936929283</v>
+        <v>-2672.117995762191</v>
       </c>
       <c r="W17">
-        <v>-51.71732724077379</v>
+        <v>-51.69253326895666</v>
       </c>
       <c r="X17">
-        <v>0.6008683091455793</v>
+        <v>0.6012509154507042</v>
       </c>
       <c r="Y17">
-        <v>-2853.43042130092</v>
+        <v>-2857.755876648326</v>
       </c>
       <c r="Z17">
-        <v>-53.41751043713026</v>
+        <v>-53.45798234733823</v>
       </c>
       <c r="AA17">
-        <v>0.4324053296474812</v>
+        <v>0.4315449247875246</v>
       </c>
       <c r="AB17">
-        <v>-2030.761468310764</v>
+        <v>-2030.194429143494</v>
       </c>
       <c r="AC17">
-        <v>-45.06397084490851</v>
+        <v>-45.05767891429267</v>
       </c>
       <c r="AD17">
-        <v>0.6307482445055035</v>
+        <v>0.6308513487898892</v>
       </c>
       <c r="AE17">
-        <v>0.02954680522172591</v>
+        <v>0.01746223940554067</v>
       </c>
       <c r="AF17">
-        <v>0.007284307951972836</v>
+        <v>0.005739691456934154</v>
       </c>
       <c r="AG17">
-        <v>1393.696465541494</v>
+        <v>1394.147048159693</v>
       </c>
       <c r="AH17">
-        <v>11.0874083392642</v>
+        <v>11.09116108164219</v>
       </c>
       <c r="AI17">
-        <v>0.0721316723846894</v>
+        <v>0.07249587623222621</v>
       </c>
     </row>
     <row r="18" spans="1:35">
@@ -2417,19 +2417,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.5893995761871338</v>
+        <v>0.3650984287261963</v>
       </c>
       <c r="C18">
-        <v>0.04900131225585937</v>
+        <v>0.02900118827819824</v>
       </c>
       <c r="D18">
-        <v>-3183.891626462746</v>
+        <v>-3184.138423025655</v>
       </c>
       <c r="E18">
-        <v>-55.22909973542353</v>
+        <v>-55.23069921868839</v>
       </c>
       <c r="F18">
-        <v>0.5745262163770452</v>
+        <v>0.5745101714721074</v>
       </c>
       <c r="G18" t="s">
         <v>34</v>
@@ -2453,22 +2453,22 @@
         <v>8</v>
       </c>
       <c r="P18">
-        <v>-5976.163061750775</v>
+        <v>-5977.391612466557</v>
       </c>
       <c r="Q18">
-        <v>-77.30564702368628</v>
+        <v>-77.31359267597487</v>
       </c>
       <c r="R18">
-        <v>0.6141919975647454</v>
+        <v>0.614112685020451</v>
       </c>
       <c r="S18">
-        <v>-2753.078780641112</v>
+        <v>-2753.084212739877</v>
       </c>
       <c r="T18">
-        <v>-52.4697892185695</v>
+        <v>-52.46984098260521</v>
       </c>
       <c r="U18">
-        <v>0.5377930372452928</v>
+        <v>0.5377921252648985</v>
       </c>
       <c r="V18">
         <v>-2374.672448759562</v>
@@ -2498,19 +2498,19 @@
         <v>0.6499048857422578</v>
       </c>
       <c r="AE18">
-        <v>0.03009446740077824</v>
+        <v>0.01534813202624262</v>
       </c>
       <c r="AF18">
-        <v>0.008225692404622316</v>
+        <v>0.003535378815016504</v>
       </c>
       <c r="AG18">
-        <v>1435.777968284338</v>
+        <v>1436.25549882897</v>
       </c>
       <c r="AH18">
-        <v>11.56019761411486</v>
+        <v>11.56322994843695</v>
       </c>
       <c r="AI18">
-        <v>0.08483931931606765</v>
+        <v>0.08483198751179712</v>
       </c>
     </row>
     <row r="19" spans="1:35">
@@ -2518,19 +2518,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.5821002960205078</v>
+        <v>0.3343992710113525</v>
       </c>
       <c r="C19">
-        <v>0.05069961547851563</v>
+        <v>0.02930045127868652</v>
       </c>
       <c r="D19">
-        <v>-3430.46197794486</v>
+        <v>-3346.855772736037</v>
       </c>
       <c r="E19">
-        <v>-57.79203614213376</v>
+        <v>-57.32081062418488</v>
       </c>
       <c r="F19">
-        <v>0.5236682461345536</v>
+        <v>0.5252403093519213</v>
       </c>
       <c r="G19" t="s">
         <v>34</v>
@@ -2545,73 +2545,73 @@
         <v>54</v>
       </c>
       <c r="M19">
+        <v>14</v>
+      </c>
+      <c r="N19">
+        <v>30</v>
+      </c>
+      <c r="O19">
         <v>57</v>
       </c>
-      <c r="N19">
-        <v>60</v>
-      </c>
-      <c r="O19">
-        <v>60</v>
-      </c>
       <c r="P19">
-        <v>-5727.337448708242</v>
+        <v>-5126.293517715487</v>
       </c>
       <c r="Q19">
-        <v>-75.67917447163548</v>
+        <v>-71.59813906600846</v>
       </c>
       <c r="R19">
-        <v>0.6302556343381609</v>
+        <v>0.6690577145351184</v>
       </c>
       <c r="S19">
-        <v>-3050.643832344674</v>
+        <v>-3029.15147474712</v>
       </c>
       <c r="T19">
-        <v>-55.23263376252009</v>
+        <v>-55.0377277396798</v>
       </c>
       <c r="U19">
-        <v>0.487835644185214</v>
+        <v>0.4914439380696666</v>
       </c>
       <c r="V19">
-        <v>-2487.25243543587</v>
+        <v>-2608.539720591887</v>
       </c>
       <c r="W19">
-        <v>-49.87236143833446</v>
+        <v>-51.07386533827146</v>
       </c>
       <c r="X19">
-        <v>0.6288376361949677</v>
+        <v>0.6107384377313774</v>
       </c>
       <c r="Y19">
-        <v>-3402.818136976578</v>
+        <v>-3480.033009366759</v>
       </c>
       <c r="Z19">
-        <v>-58.3336792682973</v>
+        <v>-58.991804594933</v>
       </c>
       <c r="AA19">
-        <v>0.3231229945862041</v>
+        <v>0.3077636749008708</v>
       </c>
       <c r="AB19">
-        <v>-2484.258036258935</v>
+        <v>-2490.261141258934</v>
       </c>
       <c r="AC19">
-        <v>-49.84233176988146</v>
+        <v>-49.90251638203162</v>
       </c>
       <c r="AD19">
-        <v>0.5482893213682214</v>
+        <v>0.5471977815225735</v>
       </c>
       <c r="AE19">
-        <v>0.02469575627928959</v>
+        <v>0.01369406045369879</v>
       </c>
       <c r="AF19">
-        <v>0.003355851241395804</v>
+        <v>0.006764943375800267</v>
       </c>
       <c r="AG19">
-        <v>1200.467331850988</v>
+        <v>955.3989576196838</v>
       </c>
       <c r="AH19">
-        <v>9.515384200922501</v>
+        <v>7.821792769076168</v>
       </c>
       <c r="AI19">
-        <v>0.1136046148327246</v>
+        <v>0.1240272452472816</v>
       </c>
     </row>
     <row r="20" spans="1:35">
@@ -2619,19 +2619,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.6073995590209961</v>
+        <v>0.336499834060669</v>
       </c>
       <c r="C20">
-        <v>0.05299949645996094</v>
+        <v>0.02810029983520508</v>
       </c>
       <c r="D20">
-        <v>-3481.605287110283</v>
+        <v>-3497.517936948739</v>
       </c>
       <c r="E20">
-        <v>-57.52508222382845</v>
+        <v>-57.66632434299125</v>
       </c>
       <c r="F20">
-        <v>0.5263234212614361</v>
+        <v>0.5235419247879707</v>
       </c>
       <c r="G20" t="s">
         <v>34</v>
@@ -2646,73 +2646,73 @@
         <v>55</v>
       </c>
       <c r="M20">
+        <v>59</v>
+      </c>
+      <c r="N20">
+        <v>37</v>
+      </c>
+      <c r="O20">
         <v>60</v>
       </c>
-      <c r="N20">
-        <v>36</v>
-      </c>
-      <c r="O20">
-        <v>56</v>
-      </c>
       <c r="P20">
-        <v>-6428.747733631957</v>
+        <v>-6433.360428246156</v>
       </c>
       <c r="Q20">
-        <v>-80.1794720214093</v>
+        <v>-80.208231673851</v>
       </c>
       <c r="R20">
-        <v>0.5849741220839282</v>
+        <v>0.5846763366191476</v>
       </c>
       <c r="S20">
-        <v>-2539.795831267483</v>
+        <v>-2582.920636267482</v>
       </c>
       <c r="T20">
-        <v>-50.39638708545964</v>
+        <v>-50.82244225012688</v>
       </c>
       <c r="U20">
-        <v>0.5736005357195626</v>
+        <v>0.5663604286515778</v>
       </c>
       <c r="V20">
-        <v>-2385.548075876251</v>
+        <v>-2384.06422692411</v>
       </c>
       <c r="W20">
-        <v>-48.8420728048703</v>
+        <v>-48.82688016783491</v>
       </c>
       <c r="X20">
-        <v>0.6440145559018773</v>
+        <v>0.6442359845259926</v>
       </c>
       <c r="Y20">
-        <v>-4107.703691469454</v>
+        <v>-4138.975907499674</v>
       </c>
       <c r="Z20">
-        <v>-64.09136986731875</v>
+        <v>-64.33487318320969</v>
       </c>
       <c r="AA20">
-        <v>0.1829095585227344</v>
+        <v>0.1766889957165199</v>
       </c>
       <c r="AB20">
-        <v>-1946.231103306272</v>
+        <v>-1948.268485806272</v>
       </c>
       <c r="AC20">
-        <v>-44.11610934008429</v>
+        <v>-44.13919443993368</v>
       </c>
       <c r="AD20">
-        <v>0.6461183340790775</v>
+        <v>0.6457478784266151</v>
       </c>
       <c r="AE20">
-        <v>0.009083893074667195</v>
+        <v>0.009617421364761654</v>
       </c>
       <c r="AF20">
-        <v>0.01784561961829202</v>
+        <v>0.004005487649964225</v>
       </c>
       <c r="AG20">
-        <v>1644.589198416171</v>
+        <v>1643.598534334771</v>
       </c>
       <c r="AH20">
-        <v>13.13279110669392</v>
+        <v>13.11918342419509</v>
       </c>
       <c r="AI20">
-        <v>0.1742470290647808</v>
+        <v>0.1762833776334469</v>
       </c>
     </row>
     <row r="21" spans="1:35">
@@ -2720,19 +2720,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.6128007411956787</v>
+        <v>0.3689999580383301</v>
       </c>
       <c r="C21">
-        <v>0.05079879760742188</v>
+        <v>0.03060388565063477</v>
       </c>
       <c r="D21">
-        <v>-3151.487172051404</v>
+        <v>-3155.642459271372</v>
       </c>
       <c r="E21">
-        <v>-55.02727496332011</v>
+        <v>-55.07254478245974</v>
       </c>
       <c r="F21">
-        <v>0.5799660147137358</v>
+        <v>0.579192625736524</v>
       </c>
       <c r="G21" t="s">
         <v>34</v>
@@ -2750,7 +2750,7 @@
         <v>3</v>
       </c>
       <c r="N21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O21">
         <v>3</v>
@@ -2765,55 +2765,55 @@
         <v>0.6226550300006011</v>
       </c>
       <c r="S21">
-        <v>-2592.406139792294</v>
+        <v>-2592.633985876495</v>
       </c>
       <c r="T21">
-        <v>-50.91567675865945</v>
+        <v>-50.91791419408787</v>
       </c>
       <c r="U21">
-        <v>0.5647679330770845</v>
+        <v>0.5647296806132267</v>
       </c>
       <c r="V21">
-        <v>-2724.403452818039</v>
+        <v>-2724.402821603837</v>
       </c>
       <c r="W21">
-        <v>-52.19581834609013</v>
+        <v>-52.19581229949235</v>
       </c>
       <c r="X21">
-        <v>0.5934485735745871</v>
+        <v>0.5934486677680642</v>
       </c>
       <c r="Y21">
-        <v>-2658.992349448478</v>
+        <v>-2664.396214656737</v>
       </c>
       <c r="Z21">
-        <v>-51.56541815450039</v>
+        <v>-51.61778971107478</v>
       </c>
       <c r="AA21">
-        <v>0.471082289307409</v>
+        <v>0.4700073708273177</v>
       </c>
       <c r="AB21">
-        <v>-1936.563165353204</v>
+        <v>-1951.708521374785</v>
       </c>
       <c r="AC21">
-        <v>-44.0063991409568</v>
+        <v>-44.1781452912499</v>
       </c>
       <c r="AD21">
-        <v>0.6478762476089969</v>
+        <v>0.6451223794734102</v>
       </c>
       <c r="AE21">
-        <v>0.02069848213893398</v>
+        <v>0.006123572533126341</v>
       </c>
       <c r="AF21">
-        <v>0.007111582359507586</v>
+        <v>0.00523063524230591</v>
       </c>
       <c r="AG21">
-        <v>1376.15087130222</v>
+        <v>1373.080515640042</v>
       </c>
       <c r="AH21">
-        <v>11.11243367415831</v>
+        <v>11.0750742866736</v>
       </c>
       <c r="AI21">
-        <v>0.06115975555098602</v>
+        <v>0.06094184837671637</v>
       </c>
     </row>
     <row r="22" spans="1:35">
@@ -2821,19 +2821,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.6044991493225098</v>
+        <v>0.3168987274169922</v>
       </c>
       <c r="C22">
-        <v>0.05550041198730469</v>
+        <v>0.02730197906494141</v>
       </c>
       <c r="D22">
-        <v>-3224.529431174031</v>
+        <v>-3225.145377968526</v>
       </c>
       <c r="E22">
-        <v>-55.65843171122716</v>
+        <v>-55.66496623906392</v>
       </c>
       <c r="F22">
-        <v>0.5693625974180223</v>
+        <v>0.5692033471036982</v>
       </c>
       <c r="G22" t="s">
         <v>34</v>
@@ -2857,13 +2857,13 @@
         <v>11</v>
       </c>
       <c r="P22">
-        <v>-5990.008216993195</v>
+        <v>-5988.770283737023</v>
       </c>
       <c r="Q22">
-        <v>-77.39514336825791</v>
+        <v>-77.38714546833359</v>
       </c>
       <c r="R22">
-        <v>0.6132981846563139</v>
+        <v>0.613378102916873</v>
       </c>
       <c r="S22">
         <v>-2690.224554707273</v>
@@ -2875,46 +2875,46 @@
         <v>0.5483454635214535</v>
       </c>
       <c r="V22">
-        <v>-2647.100586558565</v>
+        <v>-2646.751331470309</v>
       </c>
       <c r="W22">
-        <v>-51.44998140484179</v>
+        <v>-51.44658717029059</v>
       </c>
       <c r="X22">
-        <v>0.6049841596538275</v>
+        <v>0.6050362775419362</v>
       </c>
       <c r="Y22">
-        <v>-2802.458801575423</v>
+        <v>-2807.123348609862</v>
       </c>
       <c r="Z22">
-        <v>-52.93825461398801</v>
+        <v>-52.98229278362594</v>
       </c>
       <c r="AA22">
-        <v>0.4425444308077743</v>
+        <v>0.4416165749832229</v>
       </c>
       <c r="AB22">
-        <v>-1992.8549960357</v>
+        <v>-1992.857371318166</v>
       </c>
       <c r="AC22">
-        <v>-44.6414045033946</v>
+        <v>-44.64143110741597</v>
       </c>
       <c r="AD22">
-        <v>0.6376407484507423</v>
+        <v>0.6376403165550055</v>
       </c>
       <c r="AE22">
-        <v>0.06260937078413284</v>
+        <v>0.006689217396304984</v>
       </c>
       <c r="AF22">
-        <v>0.02813088444127217</v>
+        <v>0.006860874831487053</v>
       </c>
       <c r="AG22">
-        <v>1411.520047110138</v>
+        <v>1410.785506611864</v>
       </c>
       <c r="AH22">
-        <v>11.25470615434692</v>
+        <v>11.24975162269821</v>
       </c>
       <c r="AI22">
-        <v>0.06983653016888899</v>
+        <v>0.07018897701245824</v>
       </c>
     </row>
     <row r="23" spans="1:35">
@@ -2922,19 +2922,19 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.8371047019958496</v>
+        <v>0.354599142074585</v>
       </c>
       <c r="C23">
-        <v>0.06439523696899414</v>
+        <v>0.03260135650634766</v>
       </c>
       <c r="D23">
-        <v>-3164.715291124354</v>
+        <v>-3167.544293408305</v>
       </c>
       <c r="E23">
-        <v>-55.03078842176662</v>
+        <v>-55.05721080669072</v>
       </c>
       <c r="F23">
-        <v>0.5780174420135085</v>
+        <v>0.5774551881813699</v>
       </c>
       <c r="G23" t="s">
         <v>34</v>
@@ -2952,19 +2952,19 @@
         <v>7</v>
       </c>
       <c r="N23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O23">
         <v>7</v>
       </c>
       <c r="P23">
-        <v>-5980.637210332475</v>
+        <v>-5980.655135332475</v>
       </c>
       <c r="Q23">
-        <v>-77.33457965446296</v>
+        <v>-77.33469554690491</v>
       </c>
       <c r="R23">
-        <v>0.613903156328476</v>
+        <v>0.6139019991297228</v>
       </c>
       <c r="S23">
         <v>-2739.80517513406</v>
@@ -2985,13 +2985,13 @@
         <v>0.6497129410902813</v>
       </c>
       <c r="Y23">
-        <v>-2856.614041656998</v>
+        <v>-2870.741128076752</v>
       </c>
       <c r="Z23">
-        <v>-53.44730153765481</v>
+        <v>-53.57929756983337</v>
       </c>
       <c r="AA23">
-        <v>0.4317720547188036</v>
+        <v>0.4289619427568636</v>
       </c>
       <c r="AB23">
         <v>-1899.158266268147</v>
@@ -3003,19 +3003,19 @@
         <v>0.6546775508968421</v>
       </c>
       <c r="AE23">
-        <v>0.2806859542621543</v>
+        <v>0.01195576235790354</v>
       </c>
       <c r="AF23">
-        <v>0.01663491365441629</v>
+        <v>0.00455407908436422</v>
       </c>
       <c r="AG23">
-        <v>1447.383336647882</v>
+        <v>1446.799777405185</v>
       </c>
       <c r="AH23">
-        <v>11.67594179512348</v>
+        <v>11.67252464533372</v>
       </c>
       <c r="AI23">
-        <v>0.0838286415895883</v>
+        <v>0.08481081370688565</v>
       </c>
     </row>
     <row r="24" spans="1:35">
@@ -3023,19 +3023,19 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.5725973606109619</v>
+        <v>0.3572996139526367</v>
       </c>
       <c r="C24">
-        <v>0.04710173606872559</v>
+        <v>0.0268002986907959</v>
       </c>
       <c r="D24">
-        <v>-3362.290032315505</v>
+        <v>-3460.436612727105</v>
       </c>
       <c r="E24">
-        <v>-57.43121533074761</v>
+        <v>-58.05860440773197</v>
       </c>
       <c r="F24">
-        <v>0.521990463735618</v>
+        <v>0.5168277075361232</v>
       </c>
       <c r="G24" t="s">
         <v>34</v>
@@ -3050,73 +3050,73 @@
         <v>59</v>
       </c>
       <c r="M24">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="N24">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="O24">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P24">
-        <v>-5161.714714517043</v>
+        <v>-5705.858588719511</v>
       </c>
       <c r="Q24">
-        <v>-71.84507439287013</v>
+        <v>-75.53713383971827</v>
       </c>
       <c r="R24">
-        <v>0.6667709996244527</v>
+        <v>0.6316422625109892</v>
       </c>
       <c r="S24">
-        <v>-3029.437125801988</v>
+        <v>-2776.480516719958</v>
       </c>
       <c r="T24">
-        <v>-55.04032272617947</v>
+        <v>-52.69231933327625</v>
       </c>
       <c r="U24">
-        <v>0.4913959808853655</v>
+        <v>0.5338641829632255</v>
       </c>
       <c r="V24">
-        <v>-2448.537310323965</v>
+        <v>-2609.222099109859</v>
       </c>
       <c r="W24">
-        <v>-49.4826970801306</v>
+        <v>-51.08054521155641</v>
       </c>
       <c r="X24">
-        <v>0.6346149337248922</v>
+        <v>0.6106366092156499</v>
       </c>
       <c r="Y24">
-        <v>-3547.831074020944</v>
+        <v>-3671.24866656749</v>
       </c>
       <c r="Z24">
-        <v>-59.56367243564608</v>
+        <v>-60.59082988842032</v>
       </c>
       <c r="AA24">
-        <v>0.2942775145688494</v>
+        <v>0.2697277069989069</v>
       </c>
       <c r="AB24">
-        <v>-2623.929936913583</v>
+        <v>-2539.373192518708</v>
       </c>
       <c r="AC24">
-        <v>-51.22431001891176</v>
+        <v>-50.39219376568862</v>
       </c>
       <c r="AD24">
-        <v>0.5228928898745302</v>
+        <v>0.5382677759918443</v>
       </c>
       <c r="AE24">
-        <v>0.07954369551316091</v>
+        <v>0.008795569504945101</v>
       </c>
       <c r="AF24">
-        <v>0.01001822904014216</v>
+        <v>0.005154449391585682</v>
       </c>
       <c r="AG24">
-        <v>976.0394858689502</v>
+        <v>1193.907993592305</v>
       </c>
       <c r="AH24">
-        <v>7.99659539734292</v>
+        <v>9.467579783323197</v>
       </c>
       <c r="AI24">
-        <v>0.1314805679822391</v>
+        <v>0.1294533277782013</v>
       </c>
     </row>
     <row r="25" spans="1:35">
@@ -3124,19 +3124,19 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.7102997779846192</v>
+        <v>0.3276995658874512</v>
       </c>
       <c r="C25">
-        <v>0.04270229339599609</v>
+        <v>0.02700181007385254</v>
       </c>
       <c r="D25">
-        <v>-3497.963220884811</v>
+        <v>-3500.086928204547</v>
       </c>
       <c r="E25">
-        <v>-57.69791535530594</v>
+        <v>-57.71076439321133</v>
       </c>
       <c r="F25">
-        <v>0.5238954986625144</v>
+        <v>0.523328311498396</v>
       </c>
       <c r="G25" t="s">
         <v>34</v>
@@ -3151,73 +3151,73 @@
         <v>60</v>
       </c>
       <c r="M25">
+        <v>62</v>
+      </c>
+      <c r="N25">
+        <v>58</v>
+      </c>
+      <c r="O25">
         <v>61</v>
       </c>
-      <c r="N25">
-        <v>38</v>
-      </c>
-      <c r="O25">
-        <v>58</v>
-      </c>
       <c r="P25">
-        <v>-6431.759243834106</v>
+        <v>-6433.416557478553</v>
       </c>
       <c r="Q25">
-        <v>-80.19824963073762</v>
+        <v>-80.20858157004494</v>
       </c>
       <c r="R25">
-        <v>0.5847797055789903</v>
+        <v>0.5846727130387992</v>
       </c>
       <c r="S25">
-        <v>-2577.282012121113</v>
+        <v>-2535.790707121113</v>
       </c>
       <c r="T25">
-        <v>-50.76693817949939</v>
+        <v>-50.35663518466175</v>
       </c>
       <c r="U25">
-        <v>0.5673070820343777</v>
+        <v>0.5742729451980585</v>
       </c>
       <c r="V25">
-        <v>-2433.293559698547</v>
+        <v>-2433.129405190851</v>
       </c>
       <c r="W25">
-        <v>-49.32842547353957</v>
+        <v>-49.32676155182754</v>
       </c>
       <c r="X25">
-        <v>0.6368896953995724</v>
+        <v>0.6369141914958423</v>
       </c>
       <c r="Y25">
-        <v>-4090.165503628807</v>
+        <v>-4120.346310257397</v>
       </c>
       <c r="Z25">
-        <v>-63.95440175334929</v>
+        <v>-64.18992374397556</v>
       </c>
       <c r="AA25">
-        <v>0.1863981951727404</v>
+        <v>0.1803947318110799</v>
       </c>
       <c r="AB25">
-        <v>-1957.315785141484</v>
+        <v>-1977.751660974817</v>
       </c>
       <c r="AC25">
-        <v>-44.24156173940386</v>
+        <v>-44.4719199155469</v>
       </c>
       <c r="AD25">
-        <v>0.6441028151268913</v>
+        <v>0.6403869759481999</v>
       </c>
       <c r="AE25">
-        <v>0.2275783643413602</v>
+        <v>0.01582837276034678</v>
       </c>
       <c r="AF25">
-        <v>0.008311072059079366</v>
+        <v>0.004950198045438056</v>
       </c>
       <c r="AG25">
-        <v>1631.725010217338</v>
+        <v>1635.537504233032</v>
       </c>
       <c r="AH25">
-        <v>12.9966835976245</v>
+        <v>13.0213133498813</v>
       </c>
       <c r="AI25">
-        <v>0.1712970341327537</v>
+        <v>0.1735317921522543</v>
       </c>
     </row>
     <row r="26" spans="1:35">
@@ -3225,19 +3225,19 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.5190986633300781</v>
+        <v>0.3725985527038574</v>
       </c>
       <c r="C26">
-        <v>0.04580235481262207</v>
+        <v>0.03780331611633301</v>
       </c>
       <c r="D26">
-        <v>-3143.216741298991</v>
+        <v>-3142.099773208783</v>
       </c>
       <c r="E26">
-        <v>-54.9428737134895</v>
+        <v>-54.92851233496373</v>
       </c>
       <c r="F26">
-        <v>0.5817273560435812</v>
+        <v>0.5818997355285612</v>
       </c>
       <c r="G26" t="s">
         <v>34</v>
@@ -3261,13 +3261,13 @@
         <v>1</v>
       </c>
       <c r="P26">
-        <v>-5854.37271506154</v>
+        <v>-5853.844371029211</v>
       </c>
       <c r="Q26">
-        <v>-76.51387269679623</v>
+        <v>-76.51042001602926</v>
       </c>
       <c r="R26">
-        <v>0.6220545156865829</v>
+        <v>0.6220886244204988</v>
       </c>
       <c r="S26">
         <v>-2585.279056811497</v>
@@ -3279,46 +3279,46 @@
         <v>0.5659644797945337</v>
       </c>
       <c r="V26">
-        <v>-2713.436830568585</v>
+        <v>-2713.916324106478</v>
       </c>
       <c r="W26">
-        <v>-52.09065972483536</v>
+        <v>-52.09526201207244</v>
       </c>
       <c r="X26">
-        <v>0.5950850771232714</v>
+        <v>0.5950135242915531</v>
       </c>
       <c r="Y26">
-        <v>-2620.733900487784</v>
+        <v>-2627.011230474472</v>
       </c>
       <c r="Z26">
-        <v>-51.1931040325529</v>
+        <v>-51.25437767132162</v>
       </c>
       <c r="AA26">
-        <v>0.47869252979687</v>
+        <v>0.4774438646750956</v>
       </c>
       <c r="AB26">
-        <v>-1942.261203565549</v>
+        <v>-1930.447883622255</v>
       </c>
       <c r="AC26">
-        <v>-44.07109260689538</v>
+        <v>-43.9368624690277</v>
       </c>
       <c r="AD26">
-        <v>0.6468401778166477</v>
+        <v>0.6489881844611247</v>
       </c>
       <c r="AE26">
-        <v>0.02836100343560477</v>
+        <v>0.01150774245250368</v>
       </c>
       <c r="AF26">
-        <v>0.005237609180499521</v>
+        <v>0.007715772551607107</v>
       </c>
       <c r="AG26">
-        <v>1382.870526698854</v>
+        <v>1384.222933526054</v>
       </c>
       <c r="AH26">
-        <v>11.1578389216969</v>
+        <v>11.17847511409848</v>
       </c>
       <c r="AI26">
-        <v>0.05815330044614633</v>
+        <v>0.05908119761367538</v>
       </c>
     </row>
     <row r="27" spans="1:35">
@@ -3326,19 +3326,19 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.6042987823486328</v>
+        <v>0.3394987106323242</v>
       </c>
       <c r="C27">
-        <v>0.04619922637939453</v>
+        <v>0.0312009334564209</v>
       </c>
       <c r="D27">
-        <v>-3218.46960554942</v>
+        <v>-3219.35161396568</v>
       </c>
       <c r="E27">
-        <v>-55.60497088029278</v>
+        <v>-55.61328752548248</v>
       </c>
       <c r="F27">
-        <v>0.5702500163947535</v>
+        <v>0.5700725070207652</v>
       </c>
       <c r="G27" t="s">
         <v>34</v>
@@ -3362,13 +3362,13 @@
         <v>9</v>
       </c>
       <c r="P27">
-        <v>-5983.255525529416</v>
+        <v>-5983.379315556423</v>
       </c>
       <c r="Q27">
-        <v>-77.35150629127668</v>
+        <v>-77.35230646565377</v>
       </c>
       <c r="R27">
-        <v>0.6137341236321723</v>
+        <v>0.6137261320190674</v>
       </c>
       <c r="S27">
         <v>-2682.536118113974</v>
@@ -3380,46 +3380,46 @@
         <v>0.5496362543811664</v>
       </c>
       <c r="V27">
-        <v>-2637.571369617445</v>
+        <v>-2636.943075150946</v>
       </c>
       <c r="W27">
-        <v>-51.35729129945859</v>
+        <v>-51.3511740386814</v>
       </c>
       <c r="X27">
-        <v>0.6064061651707131</v>
+        <v>0.6064999229477803</v>
       </c>
       <c r="Y27">
-        <v>-2794.40596741489</v>
+        <v>-2799.070514449329</v>
       </c>
       <c r="Z27">
-        <v>-52.86214115427874</v>
+        <v>-52.90624267937886</v>
       </c>
       <c r="AA27">
-        <v>0.4441462731784978</v>
+        <v>0.4432184173539465</v>
       </c>
       <c r="AB27">
-        <v>-1994.579047071369</v>
+        <v>-1994.829046557726</v>
       </c>
       <c r="AC27">
-        <v>-44.66071032878192</v>
+        <v>-44.66350911603035</v>
       </c>
       <c r="AD27">
-        <v>0.6373272656112179</v>
+        <v>0.6372818084018652</v>
       </c>
       <c r="AE27">
-        <v>0.03081115169769131</v>
+        <v>0.01549538689217135</v>
       </c>
       <c r="AF27">
-        <v>0.006345885405822261</v>
+        <v>0.005142787282032548</v>
       </c>
       <c r="AG27">
-        <v>1410.421689786629</v>
+        <v>1410.199378707413</v>
       </c>
       <c r="AH27">
-        <v>11.24974750610921</v>
+        <v>11.24783821779525</v>
       </c>
       <c r="AI27">
-        <v>0.06931749169797838</v>
+        <v>0.06965527443904657</v>
       </c>
     </row>
     <row r="28" spans="1:35">
@@ -3427,19 +3427,19 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.6032026767730713</v>
+        <v>0.3381994724273681</v>
       </c>
       <c r="C28">
-        <v>0.04619736671447754</v>
+        <v>0.03740062713623047</v>
       </c>
       <c r="D28">
-        <v>-3162.70620690487</v>
+        <v>-3159.723948687564</v>
       </c>
       <c r="E28">
-        <v>-55.0120322559316</v>
+        <v>-54.98448643750915</v>
       </c>
       <c r="F28">
-        <v>0.5782393011372082</v>
+        <v>0.5787975098297449</v>
       </c>
       <c r="G28" t="s">
         <v>34</v>
@@ -3454,22 +3454,22 @@
         <v>63</v>
       </c>
       <c r="M28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N28">
+        <v>3</v>
+      </c>
+      <c r="O28">
         <v>4</v>
       </c>
-      <c r="O28">
-        <v>6</v>
-      </c>
       <c r="P28">
-        <v>-5978.541610094543</v>
+        <v>-5977.516419596624</v>
       </c>
       <c r="Q28">
-        <v>-77.32102954626602</v>
+        <v>-77.31439982045146</v>
       </c>
       <c r="R28">
-        <v>0.6140384436915123</v>
+        <v>0.6141046277453995</v>
       </c>
       <c r="S28">
         <v>-2732.405578421145</v>
@@ -3481,46 +3481,46 @@
         <v>0.5412638053452452</v>
       </c>
       <c r="V28">
-        <v>-2339.165033038222</v>
+        <v>-2338.500027241158</v>
       </c>
       <c r="W28">
-        <v>-48.36491531097953</v>
+        <v>-48.3580399441619</v>
       </c>
       <c r="X28">
-        <v>0.6509361049875115</v>
+        <v>0.6510353410441602</v>
       </c>
       <c r="Y28">
-        <v>-2862.530451116435</v>
+        <v>-2849.559355811244</v>
       </c>
       <c r="Z28">
-        <v>-53.50262097427036</v>
+        <v>-53.38126408967143</v>
       </c>
       <c r="AA28">
-        <v>0.4305951826802458</v>
+        <v>0.4331753488230404</v>
       </c>
       <c r="AB28">
-        <v>-1900.888361854006</v>
+        <v>-1900.638362367648</v>
       </c>
       <c r="AC28">
-        <v>-43.59917845388839</v>
+        <v>-43.5963113390072</v>
       </c>
       <c r="AD28">
-        <v>0.654362968981526</v>
+        <v>0.6544084261908786</v>
       </c>
       <c r="AE28">
-        <v>0.03489580659333904</v>
+        <v>0.01467869352835207</v>
       </c>
       <c r="AF28">
-        <v>0.004005789495034532</v>
+        <v>0.009630745424650635</v>
       </c>
       <c r="AG28">
-        <v>1447.38367216405</v>
+        <v>1447.650697937002</v>
       </c>
       <c r="AH28">
-        <v>11.67829242557365</v>
+        <v>11.6803338946683</v>
       </c>
       <c r="AI28">
-        <v>0.08429375980194491</v>
+        <v>0.08342241935551252</v>
       </c>
     </row>
     <row r="29" spans="1:35">
@@ -3528,19 +3528,19 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.60090012550354</v>
+        <v>0.3608992576599121</v>
       </c>
       <c r="C29">
-        <v>0.06020207405090332</v>
+        <v>0.03530435562133789</v>
       </c>
       <c r="D29">
-        <v>-3428.62521785807</v>
+        <v>-3428.92547831862</v>
       </c>
       <c r="E29">
-        <v>-58.03565477920584</v>
+        <v>-57.81831930356348</v>
       </c>
       <c r="F29">
-        <v>0.5115658576617703</v>
+        <v>0.5236020273886621</v>
       </c>
       <c r="G29" t="s">
         <v>34</v>
@@ -3558,70 +3558,70 @@
         <v>56</v>
       </c>
       <c r="N29">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O29">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="P29">
-        <v>-5168.742456117028</v>
+        <v>-5687.053750575797</v>
       </c>
       <c r="Q29">
-        <v>-71.89396675742012</v>
+        <v>-75.41255698208222</v>
       </c>
       <c r="R29">
-        <v>0.6663173040140242</v>
+        <v>0.6328562616882838</v>
       </c>
       <c r="S29">
-        <v>-3123.269199675002</v>
+        <v>-2899.725399258073</v>
       </c>
       <c r="T29">
-        <v>-55.88621654464544</v>
+        <v>-53.84909840710495</v>
       </c>
       <c r="U29">
-        <v>0.4756427673635493</v>
+        <v>0.5131729324136363</v>
       </c>
       <c r="V29">
-        <v>-2686.083383008602</v>
+        <v>-2654.727286896832</v>
       </c>
       <c r="W29">
-        <v>-51.82743851483114</v>
+        <v>-51.52404571553783</v>
       </c>
       <c r="X29">
-        <v>0.5991669186404157</v>
+        <v>0.6038460587979375</v>
       </c>
       <c r="Y29">
-        <v>-3646.840337854846</v>
+        <v>-3423.887592445002</v>
       </c>
       <c r="Z29">
-        <v>-60.38907465638835</v>
+        <v>-58.51399484264429</v>
       </c>
       <c r="AA29">
-        <v>0.2745829286949006</v>
+        <v>0.3189319301951352</v>
       </c>
       <c r="AB29">
-        <v>-2518.190712634871</v>
+        <v>-2479.233362417393</v>
       </c>
       <c r="AC29">
-        <v>-50.18157742274421</v>
+        <v>-49.79190057044813</v>
       </c>
       <c r="AD29">
-        <v>0.5421193695959614</v>
+        <v>0.5492029538483175</v>
       </c>
       <c r="AE29">
-        <v>0.03282598228590929</v>
+        <v>0.01596981847523139</v>
       </c>
       <c r="AF29">
-        <v>0.01725870796876238</v>
+        <v>0.006877780228039655</v>
       </c>
       <c r="AG29">
-        <v>953.847734612232</v>
+        <v>1173.074537490663</v>
       </c>
       <c r="AH29">
-        <v>7.777402664573245</v>
+        <v>9.271862338807553</v>
       </c>
       <c r="AI29">
-        <v>0.1341691843625072</v>
+        <v>0.1104804185654706</v>
       </c>
     </row>
     <row r="30" spans="1:35">
@@ -3629,19 +3629,19 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.6107999324798584</v>
+        <v>0.319597864151001</v>
       </c>
       <c r="C30">
-        <v>0.0558990478515625</v>
+        <v>0.02890024185180664</v>
       </c>
       <c r="D30">
-        <v>-3498.559309386489</v>
+        <v>-3498.78183416414</v>
       </c>
       <c r="E30">
-        <v>-57.70389406895386</v>
+        <v>-57.69958502481552</v>
       </c>
       <c r="F30">
-        <v>0.5238781146475663</v>
+        <v>0.523932632523467</v>
       </c>
       <c r="G30" t="s">
         <v>34</v>
@@ -3656,73 +3656,73 @@
         <v>65</v>
       </c>
       <c r="M30">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N30">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O30">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P30">
-        <v>-6440.492527775855</v>
+        <v>-6446.766369124206</v>
       </c>
       <c r="Q30">
-        <v>-80.25267925605883</v>
+        <v>-80.29175779072349</v>
       </c>
       <c r="R30">
-        <v>0.5842159038892688</v>
+        <v>0.5838108784284184</v>
       </c>
       <c r="S30">
-        <v>-2532.324874028238</v>
+        <v>-2533.957140694905</v>
       </c>
       <c r="T30">
-        <v>-50.32221054393614</v>
+        <v>-50.33842608480032</v>
       </c>
       <c r="U30">
-        <v>0.5748548145577501</v>
+        <v>0.5745807777144492</v>
       </c>
       <c r="V30">
-        <v>-2437.555442799409</v>
+        <v>-2430.182609466076</v>
       </c>
       <c r="W30">
-        <v>-49.37160563319173</v>
+        <v>-49.29688235036852</v>
       </c>
       <c r="X30">
-        <v>0.6362537122627424</v>
+        <v>0.6373539295985277</v>
       </c>
       <c r="Y30">
-        <v>-4094.924352177431</v>
+        <v>-4097.453881384002</v>
       </c>
       <c r="Z30">
-        <v>-63.99159594960444</v>
+        <v>-64.01135744056675</v>
       </c>
       <c r="AA30">
-        <v>0.1854515812118567</v>
+        <v>0.1849484158690353</v>
       </c>
       <c r="AB30">
-        <v>-1987.499350151509</v>
+        <v>-1985.549170151509</v>
       </c>
       <c r="AC30">
-        <v>-44.58137896197817</v>
+        <v>-44.55950145761854</v>
       </c>
       <c r="AD30">
-        <v>0.6386145613162135</v>
+        <v>0.6389691610069046</v>
       </c>
       <c r="AE30">
-        <v>0.03836856443538976</v>
+        <v>0.01449962851762181</v>
       </c>
       <c r="AF30">
-        <v>0.008714285974812816</v>
+        <v>0.005669611040912111</v>
       </c>
       <c r="AG30">
-        <v>1634.21312656054</v>
+        <v>1637.784181513194</v>
       </c>
       <c r="AH30">
-        <v>12.99307194875176</v>
+        <v>13.02074199607009</v>
       </c>
       <c r="AI30">
-        <v>0.1712101155955079</v>
+        <v>0.1715568311670912</v>
       </c>
     </row>
     <row r="31" spans="1:35">
@@ -3730,19 +3730,19 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.6203989505767822</v>
+        <v>0.3568997859954834</v>
       </c>
       <c r="C31">
-        <v>0.04920101165771484</v>
+        <v>0.03310027122497559</v>
       </c>
       <c r="D31">
-        <v>-3148.004389818391</v>
+        <v>-3145.451602025547</v>
       </c>
       <c r="E31">
-        <v>-54.99844563823567</v>
+        <v>-54.97236685269686</v>
       </c>
       <c r="F31">
-        <v>0.5807287366035396</v>
+        <v>0.5812687506453823</v>
       </c>
       <c r="G31" t="s">
         <v>34</v>
@@ -3760,19 +3760,19 @@
         <v>2</v>
       </c>
       <c r="N31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O31">
         <v>2</v>
       </c>
       <c r="P31">
-        <v>-5850.596574967688</v>
+        <v>-5851.992388761623</v>
       </c>
       <c r="Q31">
-        <v>-76.48919253703551</v>
+        <v>-76.49831624788629</v>
       </c>
       <c r="R31">
-        <v>0.622298295023169</v>
+        <v>0.6222081843407722</v>
       </c>
       <c r="S31">
         <v>-2580.698493778127</v>
@@ -3784,46 +3784,46 @@
         <v>0.5667334981539964</v>
       </c>
       <c r="V31">
-        <v>-2714.635568735997</v>
+        <v>-2714.408425878854</v>
       </c>
       <c r="W31">
-        <v>-52.10216472216867</v>
+        <v>-52.09998489326897</v>
       </c>
       <c r="X31">
-        <v>0.5949061943989201</v>
+        <v>0.5949400899853019</v>
       </c>
       <c r="Y31">
-        <v>-2630.847400749853</v>
+        <v>-2617.800944468626</v>
       </c>
       <c r="Z31">
-        <v>-51.29178687421459</v>
+        <v>-51.16445000650966</v>
       </c>
       <c r="AA31">
-        <v>0.47668078673683</v>
+        <v>0.4792759434285552</v>
       </c>
       <c r="AB31">
-        <v>-1963.243910860294</v>
+        <v>-1962.357757240503</v>
       </c>
       <c r="AC31">
-        <v>-44.30850833485928</v>
+        <v>-44.29850739291904</v>
       </c>
       <c r="AD31">
-        <v>0.6430249087047827</v>
+        <v>0.6431860373182865</v>
       </c>
       <c r="AE31">
-        <v>0.0387357246828114</v>
+        <v>0.008510116980429741</v>
       </c>
       <c r="AF31">
-        <v>0.003326871252543403</v>
+        <v>0.004778589422350052</v>
       </c>
       <c r="AG31">
-        <v>1377.298644291927</v>
+        <v>1379.002072894178</v>
       </c>
       <c r="AH31">
-        <v>11.09843985416093</v>
+        <v>11.11262726082646</v>
       </c>
       <c r="AI31">
-        <v>0.05802014154745808</v>
+        <v>0.05711479568122127</v>
       </c>
     </row>
     <row r="32" spans="1:35">
@@ -3831,19 +3831,19 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.6056002140045166</v>
+        <v>0.3459990501403808</v>
       </c>
       <c r="C32">
-        <v>0.04269990921020508</v>
+        <v>0.03090095520019531</v>
       </c>
       <c r="D32">
-        <v>-3219.420057989815</v>
+        <v>-3219.855445851046</v>
       </c>
       <c r="E32">
-        <v>-55.6146904627556</v>
+        <v>-55.61897372564265</v>
       </c>
       <c r="F32">
-        <v>0.5700268700199925</v>
+        <v>0.5699599139851533</v>
       </c>
       <c r="G32" t="s">
         <v>34</v>
@@ -3885,46 +3885,46 @@
         <v>0.5498021400593015</v>
       </c>
       <c r="V32">
-        <v>-2635.980881973147</v>
+        <v>-2637.900058008209</v>
       </c>
       <c r="W32">
-        <v>-51.34180442848837</v>
+        <v>-51.36049121657823</v>
       </c>
       <c r="X32">
-        <v>0.6066435070445213</v>
+        <v>0.6063571163655606</v>
       </c>
       <c r="Y32">
-        <v>-2800.964472240902</v>
+        <v>-2801.053462036821</v>
       </c>
       <c r="Z32">
-        <v>-52.92413884269542</v>
+        <v>-52.92497956576668</v>
       </c>
       <c r="AA32">
-        <v>0.4428416777144077</v>
+        <v>0.4428239761669994</v>
       </c>
       <c r="AB32">
-        <v>-1995.981814535874</v>
+        <v>-1996.150588011051</v>
       </c>
       <c r="AC32">
-        <v>-44.67641228361868</v>
+        <v>-44.67830108689284</v>
       </c>
       <c r="AD32">
-        <v>0.6370722015099425</v>
+        <v>0.637041513562115</v>
       </c>
       <c r="AE32">
-        <v>0.03426986891583726</v>
+        <v>0.02205675370255023</v>
       </c>
       <c r="AF32">
-        <v>0.005046535048239923</v>
+        <v>0.00662925345926023</v>
       </c>
       <c r="AG32">
-        <v>1409.745777752016</v>
+        <v>1409.552529840881</v>
       </c>
       <c r="AH32">
-        <v>11.24394337951312</v>
+        <v>11.24211757443048</v>
       </c>
       <c r="AI32">
-        <v>0.06976367376055279</v>
+        <v>0.06973424724922823</v>
       </c>
     </row>
     <row r="33" spans="1:35">
@@ -3932,19 +3932,19 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.6010989189147949</v>
+        <v>0.346299409866333</v>
       </c>
       <c r="C33">
-        <v>0.04830150604248047</v>
+        <v>0.03400096893310547</v>
       </c>
       <c r="D33">
-        <v>-3160.483824441094</v>
+        <v>-3160.491023688353</v>
       </c>
       <c r="E33">
-        <v>-54.99240837454703</v>
+        <v>-54.99250670022112</v>
       </c>
       <c r="F33">
-        <v>0.5786654464567801</v>
+        <v>0.5786670927873648</v>
       </c>
       <c r="G33" t="s">
         <v>34</v>
@@ -3959,73 +3959,73 @@
         <v>68</v>
       </c>
       <c r="M33">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O33">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P33">
-        <v>-5977.584666252851</v>
+        <v>-5977.691543984099</v>
       </c>
       <c r="Q33">
-        <v>-77.31484117718183</v>
+        <v>-77.31553235918446</v>
       </c>
       <c r="R33">
-        <v>0.6141002218906997</v>
+        <v>0.6140933220983796</v>
       </c>
       <c r="S33">
-        <v>-2731.823491487592</v>
+        <v>-2731.817174919545</v>
       </c>
       <c r="T33">
-        <v>-52.26684887658326</v>
+        <v>-52.26678845040649</v>
       </c>
       <c r="U33">
-        <v>0.5413615303487969</v>
+        <v>0.5413625908203508</v>
       </c>
       <c r="V33">
-        <v>-2340.152188691683</v>
+        <v>-2340.0909318181</v>
       </c>
       <c r="W33">
-        <v>-48.37511952121341</v>
+        <v>-48.37448637265413</v>
       </c>
       <c r="X33">
-        <v>0.650788795844072</v>
+        <v>0.6507979369532229</v>
       </c>
       <c r="Y33">
-        <v>-2850.919002641709</v>
+        <v>-2850.665695102027</v>
       </c>
       <c r="Z33">
-        <v>-53.3939978147517</v>
+        <v>-53.39162570199588</v>
       </c>
       <c r="AA33">
-        <v>0.4329048925018446</v>
+        <v>0.4329552795757365</v>
       </c>
       <c r="AB33">
-        <v>-1901.939773131636</v>
+        <v>-1902.189772617994</v>
       </c>
       <c r="AC33">
-        <v>-43.6112344830049</v>
+        <v>-43.61410061686465</v>
       </c>
       <c r="AD33">
-        <v>0.6541717916984872</v>
+        <v>0.6541263344891344</v>
       </c>
       <c r="AE33">
-        <v>0.0198358062469726</v>
+        <v>0.0243119440628234</v>
       </c>
       <c r="AF33">
-        <v>0.004949504043349404</v>
+        <v>0.001414212761523581</v>
       </c>
       <c r="AG33">
-        <v>1447.239740649609</v>
+        <v>1447.256032883778</v>
       </c>
       <c r="AH33">
-        <v>11.67556617933987</v>
+        <v>11.67541136382303</v>
       </c>
       <c r="AI33">
-        <v>0.08342221557222591</v>
+        <v>0.08339728045675036</v>
       </c>
     </row>
     <row r="34" spans="1:35">
@@ -4033,10 +4033,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>13.13959865570068</v>
+        <v>7.404010152816772</v>
       </c>
       <c r="C34">
-        <v>0.0743013858795166</v>
+        <v>0.06829066276550293</v>
       </c>
       <c r="D34">
         <v>-3413.465694698617</v>
@@ -4057,7 +4057,7 @@
         <v>69</v>
       </c>
       <c r="M34">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N34">
         <v>59</v>
@@ -4102,19 +4102,19 @@
         <v>0.4098933959086736</v>
       </c>
       <c r="AB34">
-        <v>-2551.193108788385</v>
+        <v>-2551.193108788384</v>
       </c>
       <c r="AC34">
-        <v>-50.50933684764021</v>
+        <v>-50.5093368476402</v>
       </c>
       <c r="AD34">
-        <v>0.5361185699425456</v>
+        <v>0.5361185699425457</v>
       </c>
       <c r="AE34">
-        <v>0.714283680241071</v>
+        <v>0.4831306404392013</v>
       </c>
       <c r="AF34">
-        <v>0.02288130603943808</v>
+        <v>0.01825895356145951</v>
       </c>
       <c r="AG34">
         <v>1139.180602356281</v>
@@ -4131,10 +4131,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>2.623404407501221</v>
+        <v>1.070692491531372</v>
       </c>
       <c r="C35">
-        <v>0.09800000190734863</v>
+        <v>0.04509625434875488</v>
       </c>
       <c r="D35">
         <v>-3395.653723349646</v>
@@ -4158,7 +4158,7 @@
         <v>33</v>
       </c>
       <c r="N35">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O35">
         <v>34</v>
@@ -4209,10 +4209,10 @@
         <v>0.5397834011186027</v>
       </c>
       <c r="AE35">
-        <v>1.318344503325303</v>
+        <v>0.2499222405948974</v>
       </c>
       <c r="AF35">
-        <v>0.03352308652476338</v>
+        <v>0.02202099558990892</v>
       </c>
       <c r="AG35">
         <v>1153.654501445455</v>
@@ -4229,10 +4229,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>2.167594766616821</v>
+        <v>0.7707950592041015</v>
       </c>
       <c r="C36">
-        <v>0.09750642776489257</v>
+        <v>0.03360042572021484</v>
       </c>
       <c r="D36">
         <v>-3384.619746904185</v>
@@ -4307,10 +4307,10 @@
         <v>0.5429610793776845</v>
       </c>
       <c r="AE36">
-        <v>0.400696962705287</v>
+        <v>0.1771085544707143</v>
       </c>
       <c r="AF36">
-        <v>0.01246086264097894</v>
+        <v>0.01656354334573042</v>
       </c>
       <c r="AG36">
         <v>1164.863752432975</v>
@@ -4327,10 +4327,10 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>1.706203031539917</v>
+        <v>0.5369021892547607</v>
       </c>
       <c r="C37">
-        <v>0.0794975757598877</v>
+        <v>0.02889766693115235</v>
       </c>
       <c r="D37">
         <v>-3375.836942663725</v>
@@ -4354,7 +4354,7 @@
         <v>28</v>
       </c>
       <c r="N37">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O37">
         <v>32</v>
@@ -4405,10 +4405,10 @@
         <v>0.5459299544830865</v>
       </c>
       <c r="AE37">
-        <v>0.3434977105598255</v>
+        <v>0.02238932272147122</v>
       </c>
       <c r="AF37">
-        <v>0.01898396316355023</v>
+        <v>0.007763839921260961</v>
       </c>
       <c r="AG37">
         <v>1175.954367095834</v>
@@ -4425,13 +4425,13 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>1.189100360870361</v>
+        <v>0.4797999382019043</v>
       </c>
       <c r="C38">
-        <v>0.07189779281616211</v>
+        <v>0.02640180587768555</v>
       </c>
       <c r="D38">
-        <v>-3369.880365155578</v>
+        <v>-3369.880365155579</v>
       </c>
       <c r="E38">
         <v>-57.29445196544182</v>
@@ -4458,13 +4458,13 @@
         <v>31</v>
       </c>
       <c r="P38">
-        <v>-5710.203993041485</v>
+        <v>-5710.203993041486</v>
       </c>
       <c r="Q38">
         <v>-75.56589173060479</v>
       </c>
       <c r="R38">
-        <v>0.6313617327222416</v>
+        <v>0.6313617327222415</v>
       </c>
       <c r="S38">
         <v>-3082.388158897251</v>
@@ -4503,19 +4503,19 @@
         <v>0.5486867289656133</v>
       </c>
       <c r="AE38">
-        <v>0.2186286585356712</v>
+        <v>0.0281912169176399</v>
       </c>
       <c r="AF38">
-        <v>0.01915928484691826</v>
+        <v>0.006343099672383144</v>
       </c>
       <c r="AG38">
-        <v>1187.878550624501</v>
+        <v>1187.878550624502</v>
       </c>
       <c r="AH38">
         <v>9.339493515992157</v>
       </c>
       <c r="AI38">
-        <v>0.0768262865929716</v>
+        <v>0.07682628659297157</v>
       </c>
     </row>
     <row r="39" spans="1:35">
@@ -4523,10 +4523,10 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>1.095395183563233</v>
+        <v>0.4433972835540771</v>
       </c>
       <c r="C39">
-        <v>0.06049799919128418</v>
+        <v>0.03540163040161133</v>
       </c>
       <c r="D39">
         <v>-3365.447037048581</v>
@@ -4601,10 +4601,10 @@
         <v>0.5512895227783897</v>
       </c>
       <c r="AE39">
-        <v>0.1573687970440529</v>
+        <v>0.03186551774840716</v>
       </c>
       <c r="AF39">
-        <v>0.008647206416052381</v>
+        <v>0.009583961744076896</v>
       </c>
       <c r="AG39">
         <v>1200.924026564899</v>
@@ -4621,10 +4621,10 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>1.257204580307007</v>
+        <v>0.4683994293212891</v>
       </c>
       <c r="C40">
-        <v>0.08759336471557617</v>
+        <v>0.02620077133178711</v>
       </c>
       <c r="D40">
         <v>-3361.756041380338</v>
@@ -4645,7 +4645,7 @@
         <v>75</v>
       </c>
       <c r="M40">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N40">
         <v>27</v>
@@ -4687,7 +4687,7 @@
         <v>-53.76606815347913</v>
       </c>
       <c r="AA40">
-        <v>0.4249738725268092</v>
+        <v>0.4249738725268091</v>
       </c>
       <c r="AB40">
         <v>-2454.202719899957</v>
@@ -4699,10 +4699,10 @@
         <v>0.5537542558278685</v>
       </c>
       <c r="AE40">
-        <v>0.2523444632959873</v>
+        <v>0.02228544930314003</v>
       </c>
       <c r="AF40">
-        <v>0.02979505928623742</v>
+        <v>0.007359564730461308</v>
       </c>
       <c r="AG40">
         <v>1213.789812749639</v>
@@ -4711,7 +4711,7 @@
         <v>9.545573916246532</v>
       </c>
       <c r="AI40">
-        <v>0.0764876468074122</v>
+        <v>0.07648764680741223</v>
       </c>
     </row>
     <row r="41" spans="1:35">
@@ -4719,10 +4719,10 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>1.052697706222534</v>
+        <v>0.4228004932403565</v>
       </c>
       <c r="C41">
-        <v>0.0591977596282959</v>
+        <v>0.02879862785339355</v>
       </c>
       <c r="D41">
         <v>-3358.69390524394</v>
@@ -4743,7 +4743,7 @@
         <v>76</v>
       </c>
       <c r="M41">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N41">
         <v>24</v>
@@ -4752,13 +4752,13 @@
         <v>27</v>
       </c>
       <c r="P41">
-        <v>-5771.282126829943</v>
+        <v>-5771.282126829942</v>
       </c>
       <c r="Q41">
         <v>-75.96895501999447</v>
       </c>
       <c r="R41">
-        <v>0.627418662135661</v>
+        <v>0.6274186621356612</v>
       </c>
       <c r="S41">
         <v>-3087.537764043135</v>
@@ -4797,10 +4797,10 @@
         <v>0.5561572972361972</v>
       </c>
       <c r="AE41">
-        <v>0.1806447707734649</v>
+        <v>0.008158305438347457</v>
       </c>
       <c r="AF41">
-        <v>0.01064191511916714</v>
+        <v>0.006249724751738484</v>
       </c>
       <c r="AG41">
         <v>1226.600210552959</v>
@@ -4809,7 +4809,7 @@
         <v>9.646786087855331</v>
       </c>
       <c r="AI41">
-        <v>0.07644351221388164</v>
+        <v>0.0764435122138817</v>
       </c>
     </row>
     <row r="42" spans="1:35">
@@ -4817,10 +4817,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>1.205503988265991</v>
+        <v>0.4519997119903564</v>
       </c>
       <c r="C42">
-        <v>0.08220186233520507</v>
+        <v>0.0385012149810791</v>
       </c>
       <c r="D42">
         <v>-3357.046487721422</v>
@@ -4841,7 +4841,7 @@
         <v>77</v>
       </c>
       <c r="M42">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N42">
         <v>22</v>
@@ -4895,10 +4895,10 @@
         <v>0.5583766051940846</v>
       </c>
       <c r="AE42">
-        <v>0.3288637622458465</v>
+        <v>0.03390190914468908</v>
       </c>
       <c r="AF42">
-        <v>0.02088836180466121</v>
+        <v>0.006745792212797042</v>
       </c>
       <c r="AG42">
         <v>1239.077765076023</v>
@@ -4915,10 +4915,10 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>1.056799364089966</v>
+        <v>0.4798994064331055</v>
       </c>
       <c r="C43">
-        <v>0.06439805030822754</v>
+        <v>0.02920055389404297</v>
       </c>
       <c r="D43">
         <v>-3356.249615817846</v>
@@ -4939,7 +4939,7 @@
         <v>78</v>
       </c>
       <c r="M43">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N43">
         <v>19</v>
@@ -4993,10 +4993,10 @@
         <v>0.5604863897828791</v>
       </c>
       <c r="AE43">
-        <v>0.1944312691568872</v>
+        <v>0.01983299068363532</v>
       </c>
       <c r="AF43">
-        <v>0.01266085471750924</v>
+        <v>0.006104203960228374</v>
       </c>
       <c r="AG43">
         <v>1251.254139317469</v>
@@ -5013,10 +5013,10 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>1.197699451446533</v>
+        <v>0.4640991687774658</v>
       </c>
       <c r="C44">
-        <v>0.07469544410705567</v>
+        <v>0.04300184249877929</v>
       </c>
       <c r="D44">
         <v>-3356.630947674267</v>
@@ -5037,7 +5037,7 @@
         <v>79</v>
       </c>
       <c r="M44">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N44">
         <v>17</v>
@@ -5091,10 +5091,10 @@
         <v>0.5624817419132028</v>
       </c>
       <c r="AE44">
-        <v>0.2897693525056887</v>
+        <v>0.01321111481481501</v>
       </c>
       <c r="AF44">
-        <v>0.01672356325996186</v>
+        <v>0.008185942118879264</v>
       </c>
       <c r="AG44">
         <v>1263.922691644486</v>
@@ -5111,10 +5111,10 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>1.124296140670776</v>
+        <v>0.4493983745574951</v>
       </c>
       <c r="C45">
-        <v>0.07239990234375</v>
+        <v>0.04010128974914551</v>
       </c>
       <c r="D45">
         <v>-3357.864109223679</v>
@@ -5135,13 +5135,13 @@
         <v>80</v>
       </c>
       <c r="M45">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N45">
         <v>15</v>
       </c>
       <c r="O45">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P45">
         <v>-5863.847074468371</v>
@@ -5189,10 +5189,10 @@
         <v>0.5641398004775569</v>
       </c>
       <c r="AE45">
-        <v>0.1418636996159799</v>
+        <v>0.02298331773142909</v>
       </c>
       <c r="AF45">
-        <v>0.01362581398462103</v>
+        <v>0.01346261578561642</v>
       </c>
       <c r="AG45">
         <v>1276.599659737886</v>
@@ -5209,10 +5209,10 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>1.109697008132934</v>
+        <v>0.4994988918304443</v>
       </c>
       <c r="C46">
-        <v>0.06970386505126953</v>
+        <v>0.02860116958618164</v>
       </c>
       <c r="D46">
         <v>-3359.672234801705</v>
@@ -5233,13 +5233,13 @@
         <v>81</v>
       </c>
       <c r="M46">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N46">
         <v>14</v>
       </c>
       <c r="O46">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P46">
         <v>-5889.328971988879</v>
@@ -5287,10 +5287,10 @@
         <v>0.5654945206032382</v>
       </c>
       <c r="AE46">
-        <v>0.1251394861834599</v>
+        <v>0.02891902320370874</v>
       </c>
       <c r="AF46">
-        <v>0.009180009365383652</v>
+        <v>0.005851505054595811</v>
       </c>
       <c r="AG46">
         <v>1289.134304796201</v>
@@ -5307,10 +5307,10 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.9042029857635498</v>
+        <v>0.4802004814147949</v>
       </c>
       <c r="C47">
-        <v>0.05039639472961426</v>
+        <v>0.04340119361877441</v>
       </c>
       <c r="D47">
         <v>-3361.975720863345</v>
@@ -5331,13 +5331,13 @@
         <v>82</v>
       </c>
       <c r="M47">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N47">
         <v>16</v>
       </c>
       <c r="O47">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P47">
         <v>-5915.674440660861</v>
@@ -5385,10 +5385,10 @@
         <v>0.5667661114386627</v>
       </c>
       <c r="AE47">
-        <v>0.04955708296077012</v>
+        <v>0.01746612337133363</v>
       </c>
       <c r="AF47">
-        <v>0.003595311705971203</v>
+        <v>0.01186417563149667</v>
       </c>
       <c r="AG47">
         <v>1301.844214348836</v>
@@ -5405,10 +5405,10 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.9612936019897461</v>
+        <v>0.4752992630004883</v>
       </c>
       <c r="C48">
-        <v>0.04529895782470703</v>
+        <v>0.04130110740661621</v>
       </c>
       <c r="D48">
         <v>-3364.763601068925</v>
@@ -5435,7 +5435,7 @@
         <v>18</v>
       </c>
       <c r="O48">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P48">
         <v>-5942.611319849025</v>
@@ -5483,10 +5483,10 @@
         <v>0.5680269320485558</v>
       </c>
       <c r="AE48">
-        <v>0.1740732961736528</v>
+        <v>0.02347040003495621</v>
       </c>
       <c r="AF48">
-        <v>0.007490094439658964</v>
+        <v>0.009459389522926348</v>
       </c>
       <c r="AG48">
         <v>1314.611406443018</v>
@@ -5503,10 +5503,10 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.7687001705169678</v>
+        <v>0.4448999881744385</v>
       </c>
       <c r="C49">
-        <v>0.05140042304992676</v>
+        <v>0.03809914588928223</v>
       </c>
       <c r="D49">
         <v>-3368.04834869488</v>
@@ -5533,7 +5533,7 @@
         <v>20</v>
       </c>
       <c r="O49">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P49">
         <v>-5970.077155300503</v>
@@ -5581,10 +5581,10 @@
         <v>0.5691493825292542</v>
       </c>
       <c r="AE49">
-        <v>0.04358231273531665</v>
+        <v>0.04355007165440249</v>
       </c>
       <c r="AF49">
-        <v>0.01073889604783481</v>
+        <v>0.01479542472393565</v>
       </c>
       <c r="AG49">
         <v>1327.360375225504</v>
@@ -5601,10 +5601,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.7419087409973144</v>
+        <v>0.4565989017486572</v>
       </c>
       <c r="C50">
-        <v>0.04749035835266113</v>
+        <v>0.04110035896301269</v>
       </c>
       <c r="D50">
         <v>-3371.865204426893</v>
@@ -5631,7 +5631,7 @@
         <v>21</v>
       </c>
       <c r="O50">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P50">
         <v>-5997.827156755448</v>
@@ -5679,10 +5679,10 @@
         <v>0.5701380398008042</v>
       </c>
       <c r="AE50">
-        <v>0.0314050988507263</v>
+        <v>0.01602343763278317</v>
       </c>
       <c r="AF50">
-        <v>0.007045716770098686</v>
+        <v>0.005102757477923182</v>
       </c>
       <c r="AG50">
         <v>1339.984319139405</v>
@@ -5699,10 +5699,10 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.7574992656707764</v>
+        <v>0.4601987838745117</v>
       </c>
       <c r="C51">
-        <v>0.04839854240417481</v>
+        <v>0.03150091171264648</v>
       </c>
       <c r="D51">
         <v>-3375.961625305527</v>
@@ -5729,7 +5729,7 @@
         <v>23</v>
       </c>
       <c r="O51">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P51">
         <v>-6024.482100211865</v>
@@ -5777,10 +5777,10 @@
         <v>0.5710178967266869</v>
       </c>
       <c r="AE51">
-        <v>0.03117277763739829</v>
+        <v>0.02935489549833964</v>
       </c>
       <c r="AF51">
-        <v>0.009368019441306526</v>
+        <v>0.01129193063079448</v>
       </c>
       <c r="AG51">
         <v>1351.953060717794</v>
@@ -5797,10 +5797,10 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.7430953502655029</v>
+        <v>0.4606974124908447</v>
       </c>
       <c r="C52">
-        <v>0.04900250434875488</v>
+        <v>0.04310264587402344</v>
       </c>
       <c r="D52">
         <v>-3380.253378369308</v>
@@ -5827,7 +5827,7 @@
         <v>25</v>
       </c>
       <c r="O52">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P52">
         <v>-6051.337864564777</v>
@@ -5875,10 +5875,10 @@
         <v>0.5717891114666352</v>
       </c>
       <c r="AE52">
-        <v>0.04816372785381379</v>
+        <v>0.02365610651083001</v>
       </c>
       <c r="AF52">
-        <v>0.003604841372640637</v>
+        <v>0.009298021960346755</v>
       </c>
       <c r="AG52">
         <v>1363.835196012741</v>
@@ -5895,10 +5895,10 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.7728943347930908</v>
+        <v>0.4294986724853516</v>
       </c>
       <c r="C53">
-        <v>0.05280251502990722</v>
+        <v>0.118303108215332</v>
       </c>
       <c r="D53">
         <v>-3384.824248665328</v>
@@ -5973,10 +5973,10 @@
         <v>0.5724556162410432</v>
       </c>
       <c r="AE53">
-        <v>0.04248854852924622</v>
+        <v>0.01924010455811003</v>
       </c>
       <c r="AF53">
-        <v>0.008675378533760408</v>
+        <v>0.1675851517764141</v>
       </c>
       <c r="AG53">
         <v>1375.65954102586</v>
@@ -5993,19 +5993,19 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>2.156999778747559</v>
+        <v>1.653298091888428</v>
       </c>
       <c r="C54">
-        <v>0.04530024528503418</v>
+        <v>0.04260149002075195</v>
       </c>
       <c r="D54">
-        <v>-1.360700388185078E+30</v>
+        <v>-8.502483033934E+29</v>
       </c>
       <c r="E54">
-        <v>-788198026650423</v>
+        <v>-645007779556010.4</v>
       </c>
       <c r="F54">
-        <v>-2.606833032565493E+26</v>
+        <v>-1.551882185398839E+26</v>
       </c>
       <c r="G54" t="s">
         <v>36</v>
@@ -6026,64 +6026,64 @@
         <v>72</v>
       </c>
       <c r="P54">
-        <v>-5692.320400005896</v>
+        <v>-5778.774087770721</v>
       </c>
       <c r="Q54">
-        <v>-75.44746781705729</v>
+        <v>-76.0182483866257</v>
       </c>
       <c r="R54">
-        <v>0.6325162583324253</v>
+        <v>0.626934997541001</v>
       </c>
       <c r="S54">
-        <v>-1.04242416407302E+30</v>
+        <v>-1.765429463240492E+29</v>
       </c>
       <c r="T54">
-        <v>-1020991755144487</v>
+        <v>-420170139733952.6</v>
       </c>
       <c r="U54">
-        <v>-1.750097782040601E+26</v>
+        <v>-2.963931856581451E+25</v>
       </c>
       <c r="V54">
-        <v>-3.53531639799301E+29</v>
+        <v>-1.292462016318833E+30</v>
       </c>
       <c r="W54">
-        <v>-594585267055366.1</v>
+        <v>-1136864994763597</v>
       </c>
       <c r="X54">
-        <v>-5.275606015630778E+25</v>
+        <v>-1.928687455566006E+26</v>
       </c>
       <c r="Y54">
-        <v>-5.407546137053069E+30</v>
+        <v>-2.782236554324118E+30</v>
       </c>
       <c r="Z54">
-        <v>-2325413111052114</v>
+        <v>-1668003763282361</v>
       </c>
       <c r="AA54">
-        <v>-1.075650677922379E+27</v>
+        <v>-5.534330285770041E+26</v>
       </c>
       <c r="AB54">
-        <v>-5308.856892239351</v>
+        <v>-4359.279300883026</v>
       </c>
       <c r="AC54">
-        <v>-72.86190288648349</v>
+        <v>-66.02483851463043</v>
       </c>
       <c r="AD54">
-        <v>0.03469474001835082</v>
+        <v>0.2073556842296982</v>
       </c>
       <c r="AE54">
-        <v>0.1110466741126915</v>
+        <v>0.5045264064724457</v>
       </c>
       <c r="AF54">
-        <v>0.005289303404736954</v>
+        <v>0.02505521157243873</v>
       </c>
       <c r="AG54">
-        <v>2.058915260544007E+30</v>
+        <v>1.079616119981939E+30</v>
       </c>
       <c r="AH54">
-        <v>859909448121985.2</v>
+        <v>658948607787910.1</v>
       </c>
       <c r="AI54">
-        <v>4.124698976365166E+26</v>
+        <v>2.116355563083027E+26</v>
       </c>
     </row>
     <row r="55" spans="1:35">
@@ -6091,10 +6091,10 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.9086019992828369</v>
+        <v>1.051306247711182</v>
       </c>
       <c r="C55">
-        <v>0.06489777565002441</v>
+        <v>0.1273947238922119</v>
       </c>
       <c r="D55">
         <v>-3409.934944179974</v>
@@ -6118,7 +6118,7 @@
         <v>52</v>
       </c>
       <c r="N55">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O55">
         <v>53</v>
@@ -6169,10 +6169,10 @@
         <v>0.5361216020197488</v>
       </c>
       <c r="AE55">
-        <v>0.03636265135995694</v>
+        <v>0.4472443398375517</v>
       </c>
       <c r="AF55">
-        <v>0.01294866126760032</v>
+        <v>0.153674895230004</v>
       </c>
       <c r="AG55">
         <v>1140.670582025943</v>
@@ -6189,10 +6189,10 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0.926398754119873</v>
+        <v>0.469299840927124</v>
       </c>
       <c r="C56">
-        <v>0.0528019905090332</v>
+        <v>0.05200052261352539</v>
       </c>
       <c r="D56">
         <v>-3409.930852119293</v>
@@ -6216,7 +6216,7 @@
         <v>51</v>
       </c>
       <c r="N56">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O56">
         <v>52</v>
@@ -6267,10 +6267,10 @@
         <v>0.536124633818553</v>
       </c>
       <c r="AE56">
-        <v>0.06546657037259897</v>
+        <v>0.01791789714337101</v>
       </c>
       <c r="AF56">
-        <v>0.005436332213163756</v>
+        <v>0.01959090819124608</v>
       </c>
       <c r="AG56">
         <v>1140.688618928523</v>
@@ -6287,10 +6287,10 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.8005049228668213</v>
+        <v>0.4677992820739746</v>
       </c>
       <c r="C57">
-        <v>0.04989461898803711</v>
+        <v>0.04719977378845215</v>
       </c>
       <c r="D57">
         <v>-3409.926761165685</v>
@@ -6314,7 +6314,7 @@
         <v>50</v>
       </c>
       <c r="N57">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O57">
         <v>51</v>
@@ -6365,10 +6365,10 @@
         <v>0.5361276653389904</v>
       </c>
       <c r="AE57">
-        <v>0.03701158055879602</v>
+        <v>0.03218049542482342</v>
       </c>
       <c r="AF57">
-        <v>0.004994446878625906</v>
+        <v>0.01336302948385638</v>
       </c>
       <c r="AG57">
         <v>1140.706655315732</v>
@@ -6385,10 +6385,10 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.8184992790222168</v>
+        <v>0.4803000926971436</v>
       </c>
       <c r="C58">
-        <v>0.0440007209777832</v>
+        <v>0.0403017520904541</v>
       </c>
       <c r="D58">
         <v>-3409.922671319136</v>
@@ -6412,7 +6412,7 @@
         <v>49</v>
       </c>
       <c r="N58">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O58">
         <v>50</v>
@@ -6463,10 +6463,10 @@
         <v>0.5361306965810917</v>
       </c>
       <c r="AE58">
-        <v>0.05574069239193784</v>
+        <v>0.04347327221732143</v>
       </c>
       <c r="AF58">
-        <v>0.005374839655281615</v>
+        <v>0.007073991969399344</v>
       </c>
       <c r="AG58">
         <v>1140.724691187525</v>
@@ -6483,10 +6483,10 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.7970040798187256</v>
+        <v>0.4676988124847412</v>
       </c>
       <c r="C59">
-        <v>0.0446983814239502</v>
+        <v>0.04760136604309082</v>
       </c>
       <c r="D59">
         <v>-3409.918582579528</v>
@@ -6510,7 +6510,7 @@
         <v>48</v>
       </c>
       <c r="N59">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O59">
         <v>49</v>
@@ -6561,10 +6561,10 @@
         <v>0.5361337275448881</v>
       </c>
       <c r="AE59">
-        <v>0.02697205129399869</v>
+        <v>0.03265057411946012</v>
       </c>
       <c r="AF59">
-        <v>0.007058350948573891</v>
+        <v>0.01430933245279735</v>
       </c>
       <c r="AG59">
         <v>1140.742726543926</v>
@@ -6581,10 +6581,10 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.7784983158111572</v>
+        <v>0.5004991531372071</v>
       </c>
       <c r="C60">
-        <v>0.04770164489746094</v>
+        <v>0.04260025024414062</v>
       </c>
       <c r="D60">
         <v>-3409.914494946706</v>
@@ -6608,19 +6608,19 @@
         <v>47</v>
       </c>
       <c r="N60">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O60">
         <v>48</v>
       </c>
       <c r="P60">
-        <v>-5662.039683784483</v>
+        <v>-5662.039683784484</v>
       </c>
       <c r="Q60">
-        <v>-75.24652605791501</v>
+        <v>-75.24652605791502</v>
       </c>
       <c r="R60">
-        <v>0.6344711150719383</v>
+        <v>0.6344711150719382</v>
       </c>
       <c r="S60">
         <v>-3095.754267181602</v>
@@ -6659,19 +6659,19 @@
         <v>0.5361367582304106</v>
       </c>
       <c r="AE60">
-        <v>0.05089264187429147</v>
+        <v>0.02794274703196992</v>
       </c>
       <c r="AF60">
-        <v>0.008430185175794688</v>
+        <v>0.0137527451362234</v>
       </c>
       <c r="AG60">
         <v>1140.760761384978</v>
       </c>
       <c r="AH60">
-        <v>8.937277507237313</v>
+        <v>8.937277507237319</v>
       </c>
       <c r="AI60">
-        <v>0.07818392518612893</v>
+        <v>0.07818392518612892</v>
       </c>
     </row>
     <row r="61" spans="1:35">
@@ -6679,10 +6679,10 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.818200159072876</v>
+        <v>0.4705991268157959</v>
       </c>
       <c r="C61">
-        <v>0.04910035133361816</v>
+        <v>0.05750136375427246</v>
       </c>
       <c r="D61">
         <v>-3409.910408420509</v>
@@ -6706,7 +6706,7 @@
         <v>46</v>
       </c>
       <c r="N61">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O61">
         <v>47</v>
@@ -6757,10 +6757,10 @@
         <v>0.5361397886376901</v>
       </c>
       <c r="AE61">
-        <v>0.03882244826859377</v>
+        <v>0.03505559146259379</v>
       </c>
       <c r="AF61">
-        <v>0.01052524606181594</v>
+        <v>0.01569422170842003</v>
       </c>
       <c r="AG61">
         <v>1140.778795710726</v>
@@ -6777,10 +6777,10 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.8051988124847412</v>
+        <v>0.4796989917755127</v>
       </c>
       <c r="C62">
-        <v>0.04890165328979492</v>
+        <v>0.03720436096191406</v>
       </c>
       <c r="D62">
         <v>-3409.906323000771</v>
@@ -6804,7 +6804,7 @@
         <v>45</v>
       </c>
       <c r="N62">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O62">
         <v>46</v>
@@ -6855,10 +6855,10 @@
         <v>0.5361428187667572</v>
       </c>
       <c r="AE62">
-        <v>0.0363194114795738</v>
+        <v>0.0180740172187863</v>
       </c>
       <c r="AF62">
-        <v>0.006830902100714472</v>
+        <v>0.0104903726474931</v>
       </c>
       <c r="AG62">
         <v>1140.796829521221</v>
@@ -6875,10 +6875,10 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0.8478002071380615</v>
+        <v>0.4870997905731201</v>
       </c>
       <c r="C63">
-        <v>0.04509835243225098</v>
+        <v>0.0330007553100586</v>
       </c>
       <c r="D63">
         <v>-3409.902238687336</v>
@@ -6902,7 +6902,7 @@
         <v>44</v>
       </c>
       <c r="N63">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O63">
         <v>45</v>
@@ -6953,10 +6953,10 @@
         <v>0.5361458486176434</v>
       </c>
       <c r="AE63">
-        <v>0.068589571485064</v>
+        <v>0.01657791262848878</v>
       </c>
       <c r="AF63">
-        <v>0.006321390114371011</v>
+        <v>0.009955611423929804</v>
       </c>
       <c r="AG63">
         <v>1140.814862816506</v>
@@ -6973,10 +6973,10 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.8076988220214844</v>
+        <v>0.4699002265930176</v>
       </c>
       <c r="C64">
-        <v>0.0508018970489502</v>
+        <v>0.06240167617797852</v>
       </c>
       <c r="D64">
         <v>-3409.898155480036</v>
@@ -7000,7 +7000,7 @@
         <v>43</v>
       </c>
       <c r="N64">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O64">
         <v>44</v>
@@ -7051,10 +7051,10 @@
         <v>0.5361488781903794</v>
       </c>
       <c r="AE64">
-        <v>0.04101413703734948</v>
+        <v>0.03429563959201933</v>
       </c>
       <c r="AF64">
-        <v>0.006447131839751553</v>
+        <v>0.03623965790634077</v>
       </c>
       <c r="AG64">
         <v>1140.832895596632</v>
@@ -7071,10 +7071,10 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0.833402156829834</v>
+        <v>0.490900182723999</v>
       </c>
       <c r="C65">
-        <v>0.03779926300048828</v>
+        <v>0.03730072975158692</v>
       </c>
       <c r="D65">
         <v>-3409.8940733787</v>
@@ -7098,7 +7098,7 @@
         <v>42</v>
       </c>
       <c r="N65">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O65">
         <v>43</v>
@@ -7149,10 +7149,10 @@
         <v>0.5361519074849959</v>
       </c>
       <c r="AE65">
-        <v>0.1504260894114995</v>
+        <v>0.03356359963031422</v>
       </c>
       <c r="AF65">
-        <v>0.005819479861765774</v>
+        <v>0.007158969491849599</v>
       </c>
       <c r="AG65">
         <v>1140.850927861654</v>
@@ -7169,10 +7169,10 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0.9935999393463135</v>
+        <v>0.4716001033782959</v>
       </c>
       <c r="C66">
-        <v>0.04010791778564453</v>
+        <v>0.04570050239562988</v>
       </c>
       <c r="D66">
         <v>-3409.88999238318</v>
@@ -7196,7 +7196,7 @@
         <v>41</v>
       </c>
       <c r="N66">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O66">
         <v>42</v>
@@ -7247,10 +7247,10 @@
         <v>0.5361549365015241</v>
       </c>
       <c r="AE66">
-        <v>0.1933887185987575</v>
+        <v>0.02070184742861387</v>
       </c>
       <c r="AF66">
-        <v>0.004171547464103411</v>
+        <v>0.01425698351030115</v>
       </c>
       <c r="AG66">
         <v>1140.868959611609</v>
@@ -7267,10 +7267,10 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.7830000400543213</v>
+        <v>0.4951987743377685</v>
       </c>
       <c r="C67">
-        <v>0.04269952774047851</v>
+        <v>0.03410067558288574</v>
       </c>
       <c r="D67">
         <v>-3409.885912493309</v>
@@ -7294,7 +7294,7 @@
         <v>40</v>
       </c>
       <c r="N67">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O67">
         <v>41</v>
@@ -7345,10 +7345,10 @@
         <v>0.5361579652399948</v>
       </c>
       <c r="AE67">
-        <v>0.1127185594300268</v>
+        <v>0.02812404221373853</v>
       </c>
       <c r="AF67">
-        <v>0.00553779293454904</v>
+        <v>0.01087815392896565</v>
       </c>
       <c r="AG67">
         <v>1140.886990846549</v>
@@ -7365,10 +7365,10 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.7714968681335449</v>
+        <v>0.4558996200561524</v>
       </c>
       <c r="C68">
-        <v>0.05319962501525879</v>
+        <v>0.04730238914489746</v>
       </c>
       <c r="D68">
         <v>-3409.881833708913</v>
@@ -7392,7 +7392,7 @@
         <v>39</v>
       </c>
       <c r="N68">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O68">
         <v>40</v>
@@ -7443,10 +7443,10 @@
         <v>0.536160993700439</v>
       </c>
       <c r="AE68">
-        <v>0.06061783952784058</v>
+        <v>0.03472721587100254</v>
       </c>
       <c r="AF68">
-        <v>0.01140839686378542</v>
+        <v>0.007521054044072003</v>
       </c>
       <c r="AG68">
         <v>1140.905021566527</v>
@@ -7463,10 +7463,10 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0.9723016738891601</v>
+        <v>0.4683001518249512</v>
       </c>
       <c r="C69">
-        <v>0.04269919395446777</v>
+        <v>0.03329987525939941</v>
       </c>
       <c r="D69">
         <v>-3409.877756029833</v>
@@ -7490,7 +7490,7 @@
         <v>38</v>
       </c>
       <c r="N69">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O69">
         <v>39</v>
@@ -7541,10 +7541,10 @@
         <v>0.5361640218828876</v>
       </c>
       <c r="AE69">
-        <v>0.1235978873752792</v>
+        <v>0.02589522993097743</v>
       </c>
       <c r="AF69">
-        <v>0.005624961945998543</v>
+        <v>0.006431772724729913</v>
       </c>
       <c r="AG69">
         <v>1140.92305177159</v>
@@ -7561,10 +7561,10 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.8703008651733398</v>
+        <v>0.4554990768432617</v>
       </c>
       <c r="C70">
-        <v>0.04810080528259277</v>
+        <v>0.04160399436950683</v>
       </c>
       <c r="D70">
         <v>-3409.873679455913</v>
@@ -7588,7 +7588,7 @@
         <v>37</v>
       </c>
       <c r="N70">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O70">
         <v>38</v>
@@ -7639,10 +7639,10 @@
         <v>0.5361670497873716</v>
       </c>
       <c r="AE70">
-        <v>0.09463767892017828</v>
+        <v>0.02623826582855772</v>
       </c>
       <c r="AF70">
-        <v>0.005598574995193733</v>
+        <v>0.01844358076862202</v>
       </c>
       <c r="AG70">
         <v>1140.941081461782</v>
@@ -7659,19 +7659,19 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.795100212097168</v>
+        <v>0.4392989635467529</v>
       </c>
       <c r="C71">
-        <v>0.05170135498046875</v>
+        <v>0.04270238876342773</v>
       </c>
       <c r="D71">
         <v>-3409.869603986978</v>
       </c>
       <c r="E71">
-        <v>-57.70587326449786</v>
+        <v>-57.70587326449785</v>
       </c>
       <c r="F71">
-        <v>0.5294415438381902</v>
+        <v>0.5294415438381903</v>
       </c>
       <c r="G71" t="s">
         <v>36</v>
@@ -7686,19 +7686,19 @@
         <v>36</v>
       </c>
       <c r="N71">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O71">
         <v>37</v>
       </c>
       <c r="P71">
-        <v>-5662.385127288036</v>
+        <v>-5662.385127288035</v>
       </c>
       <c r="Q71">
-        <v>-75.24882143454498</v>
+        <v>-75.24882143454496</v>
       </c>
       <c r="R71">
-        <v>0.6344488139956987</v>
+        <v>0.6344488139956989</v>
       </c>
       <c r="S71">
         <v>-3095.710421898499</v>
@@ -7737,19 +7737,19 @@
         <v>0.5361700774139216</v>
       </c>
       <c r="AE71">
-        <v>0.07717455427311885</v>
+        <v>0.0218948023823806</v>
       </c>
       <c r="AF71">
-        <v>0.01674583617590969</v>
+        <v>0.01935957880466193</v>
       </c>
       <c r="AG71">
-        <v>1140.959110637158</v>
+        <v>1140.959110637157</v>
       </c>
       <c r="AH71">
-        <v>8.938780384856225</v>
+        <v>8.938780384856219</v>
       </c>
       <c r="AI71">
-        <v>0.07816965680342854</v>
+        <v>0.07816965680342856</v>
       </c>
     </row>
     <row r="72" spans="1:35">
@@ -7757,10 +7757,10 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0.8037966728210449</v>
+        <v>0.4324999332427978</v>
       </c>
       <c r="C72">
-        <v>0.03820242881774902</v>
+        <v>0.04100027084350586</v>
       </c>
       <c r="D72">
         <v>-3409.86552962287</v>
@@ -7784,7 +7784,7 @@
         <v>35</v>
       </c>
       <c r="N72">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O72">
         <v>36</v>
@@ -7835,10 +7835,10 @@
         <v>0.5361731047625689</v>
       </c>
       <c r="AE72">
-        <v>0.02143252707477576</v>
+        <v>0.02691271430899127</v>
       </c>
       <c r="AF72">
-        <v>0.005844878428770583</v>
+        <v>0.01406081394167321</v>
       </c>
       <c r="AG72">
         <v>1140.977139297764</v>
@@ -7855,10 +7855,10 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.6102968215942383</v>
+        <v>0.3862994194030762</v>
       </c>
       <c r="C73">
-        <v>0.0196023941040039</v>
+        <v>0.03410077095031738</v>
       </c>
       <c r="D73">
         <v>-3409.861456363427</v>
@@ -7867,7 +7867,7 @@
         <v>-57.70576035080218</v>
       </c>
       <c r="F73">
-        <v>0.5294444074865239</v>
+        <v>0.529444407486524</v>
       </c>
       <c r="G73" t="s">
         <v>36</v>
@@ -7882,7 +7882,7 @@
         <v>34</v>
       </c>
       <c r="N73">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O73">
         <v>35</v>
@@ -7921,7 +7921,7 @@
         <v>-54.4034581225762</v>
       </c>
       <c r="AA73">
-        <v>0.4112593347849562</v>
+        <v>0.4112593347849564</v>
       </c>
       <c r="AB73">
         <v>-2550.876537592345</v>
@@ -7933,19 +7933,19 @@
         <v>0.536176131833344</v>
       </c>
       <c r="AE73">
-        <v>0.07159161480508873</v>
+        <v>0.07140551680767092</v>
       </c>
       <c r="AF73">
-        <v>0.005286723523292954</v>
+        <v>0.01562432727303249</v>
       </c>
       <c r="AG73">
         <v>1140.995167443647</v>
       </c>
       <c r="AH73">
-        <v>8.939053568427438</v>
+        <v>8.93905356842744</v>
       </c>
       <c r="AI73">
-        <v>0.07816706340925297</v>
+        <v>0.07816706340925293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>